<commit_message>
Changes in EditCustomer,UpdateAddCustStatus in Excel and data files
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/bin/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/bin/guru99/DataFiles/Guru99_testdata.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{8BFC7396-AB87-4D52-B24E-7FD7D002E97F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5441AD-8745-4A45-A256-BEAF8AF0D3A3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="2" windowHeight="12648" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" r:id="rId1" sheetId="6"/>
-    <sheet name="LoginLogout" r:id="rId2" sheetId="1"/>
-    <sheet name="NewCust" r:id="rId3" sheetId="2"/>
-    <sheet name="EditCust" r:id="rId4" sheetId="3"/>
-    <sheet name="DeleteCust" r:id="rId5" sheetId="7"/>
-    <sheet name="NewAcct" r:id="rId6" sheetId="8"/>
-    <sheet name="EditAcct" r:id="rId7" sheetId="9"/>
-    <sheet name="DeleteAcct" r:id="rId8" sheetId="10"/>
-    <sheet name="Deposit" r:id="rId9" sheetId="18"/>
-    <sheet name="Withdrawal" r:id="rId10" sheetId="12"/>
-    <sheet name="FundTransfer" r:id="rId11" sheetId="13"/>
-    <sheet name="BalEnquiry" r:id="rId12" sheetId="17"/>
-    <sheet name="MiniStat" r:id="rId13" sheetId="15"/>
-    <sheet name="CustStat" r:id="rId14" sheetId="16"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
+    <sheet name="LoginLogout" sheetId="1" r:id="rId2"/>
+    <sheet name="NewCust" sheetId="2" r:id="rId3"/>
+    <sheet name="EditCust" sheetId="3" r:id="rId4"/>
+    <sheet name="DeleteCust" sheetId="7" r:id="rId5"/>
+    <sheet name="NewAcct" sheetId="8" r:id="rId6"/>
+    <sheet name="EditAcct" sheetId="9" r:id="rId7"/>
+    <sheet name="DeleteAcct" sheetId="10" r:id="rId8"/>
+    <sheet name="Deposit" sheetId="18" r:id="rId9"/>
+    <sheet name="Withdrawal" sheetId="12" r:id="rId10"/>
+    <sheet name="FundTransfer" sheetId="13" r:id="rId11"/>
+    <sheet name="BalEnquiry" sheetId="17" r:id="rId12"/>
+    <sheet name="MiniStat" sheetId="15" r:id="rId13"/>
+    <sheet name="CustStat" sheetId="16" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">NewAcct!$F$1:$F$27</definedName>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">NewCust!$M$1:$M$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">NewAcct!$F$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewCust!$M$1:$M$54</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,7 +42,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C24" shapeId="0" xr:uid="{C91B75FE-20C6-4B1B-94B5-DE09A4978240}">
+    <comment ref="C24" authorId="0" shapeId="0" xr:uid="{C91B75FE-20C6-4B1B-94B5-DE09A4978240}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C2" shapeId="0" xr:uid="{5314E864-4DAD-48A0-9132-A0FFD5A6ECD7}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{5314E864-4DAD-48A0-9132-A0FFD5A6ECD7}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="D3" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="D3" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -178,7 +178,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="F3" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +212,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C2" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +246,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="D2" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="617">
   <si>
     <t>testcaseID</t>
   </si>
@@ -2054,9 +2054,6 @@
   </si>
   <si>
     <t>34355</t>
-  </si>
-  <si>
-    <t>Fail - Customer could not be added !!</t>
   </si>
   <si>
     <t>59449</t>
@@ -2135,7 +2132,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2243,7 +2239,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="184">
+  <fills count="160">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3036,136 +3032,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="240">
+  <borders count="192">
     <border>
       <left/>
       <right/>
@@ -6020,711 +5896,291 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="5" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="7" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="8" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="10" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="21" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="26" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="27" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="38" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="28" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="29" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="30" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="6" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="9" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="11" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="12" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="13" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="14" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="15" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="16" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="17" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="18" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="19" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="20" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="22" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="23" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="24" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="25" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="37" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="31" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="32" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="33" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="34" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="35" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="36" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="39" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="252">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="40" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="41" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="42" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="43" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="44" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="45" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="46" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="47" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="48" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="9" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="49" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="50" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="51" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="52" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="53" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="36" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="54" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="55" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="56" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="57" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="59" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="26" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="26" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="26" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="58" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="60" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="61" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="62" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="63" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="64" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="65" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="66" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="67" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="68" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="69" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="70" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="71" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="72" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="73" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="74" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="75" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="76" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="77" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="78" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="79" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="80" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="81" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="83" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="84" fillId="53" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="85" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="86" fillId="55" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="87" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="88" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="89" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="90" fillId="59" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="91" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="92" fillId="61" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="93" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="94" fillId="63" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="95" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="96" fillId="65" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="97" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="98" fillId="67" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="99" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="100" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="101" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="102" fillId="71" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="103" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="104" fillId="73" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="105" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="106" fillId="75" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="107" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="108" fillId="77" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="109" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="110" fillId="79" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="111" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="112" fillId="81" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="113" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="114" fillId="83" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="115" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="116" fillId="85" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="117" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="118" fillId="87" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="119" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="120" fillId="89" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="121" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="122" fillId="91" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="123" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="124" fillId="93" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="125" fillId="94" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="126" fillId="95" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="127" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="128" fillId="97" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="129" fillId="98" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="130" fillId="99" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="131" fillId="100" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="132" fillId="101" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="133" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="134" fillId="103" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="135" fillId="104" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="136" fillId="105" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="137" fillId="106" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="138" fillId="107" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="139" fillId="108" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="140" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="140" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="140" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="140" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="141" fillId="109" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="142" fillId="110" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="143" fillId="111" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="144" fillId="112" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="145" fillId="113" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="146" fillId="114" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="147" fillId="115" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="148" fillId="116" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="149" fillId="117" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="150" fillId="118" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="151" fillId="119" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="152" fillId="120" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="153" fillId="121" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="154" fillId="122" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="155" fillId="123" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="156" fillId="124" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="157" fillId="125" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="158" fillId="126" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="159" fillId="127" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="160" fillId="128" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="161" fillId="129" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="162" fillId="130" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="163" fillId="131" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="164" fillId="132" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="165" fillId="133" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="166" fillId="134" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="167" fillId="135" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="168" fillId="136" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="169" fillId="137" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="170" fillId="138" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="171" fillId="139" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="172" fillId="140" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="173" fillId="141" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="174" fillId="142" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="175" fillId="143" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="176" fillId="144" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="177" fillId="145" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="178" fillId="146" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="179" fillId="147" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="180" fillId="148" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="181" fillId="149" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="182" fillId="150" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="183" fillId="151" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="184" fillId="152" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="185" fillId="153" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="186" fillId="154" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="187" fillId="155" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="188" fillId="156" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="189" fillId="157" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="190" fillId="158" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="191" fillId="159" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="58" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="69" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="71" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="72" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="73" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="74" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="75" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="76" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="77" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="78" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="79" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="80" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="81" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="83" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="84" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="54" borderId="85" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="55" borderId="86" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="87" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="88" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="89" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="90" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="91" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="92" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="62" borderId="93" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="94" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="95" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="65" borderId="96" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="66" borderId="97" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="67" borderId="98" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="68" borderId="99" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="69" borderId="100" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="70" borderId="101" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="71" borderId="102" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="72" borderId="103" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="73" borderId="104" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="74" borderId="105" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="75" borderId="106" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="76" borderId="107" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="77" borderId="108" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="78" borderId="109" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="79" borderId="110" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="80" borderId="111" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="81" borderId="112" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="82" borderId="113" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="83" borderId="114" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="84" borderId="115" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="85" borderId="116" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="86" borderId="117" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="87" borderId="118" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="88" borderId="119" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="89" borderId="120" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="90" borderId="121" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="91" borderId="122" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="92" borderId="123" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="93" borderId="124" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="94" borderId="125" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="95" borderId="126" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="96" borderId="127" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="97" borderId="128" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="98" borderId="129" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="99" borderId="130" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="100" borderId="131" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="101" borderId="132" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="102" borderId="133" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="103" borderId="134" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="104" borderId="135" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="105" borderId="136" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="106" borderId="137" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="107" borderId="138" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="108" borderId="139" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="140" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="140" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="140" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="140" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="109" borderId="141" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="110" borderId="142" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="111" borderId="143" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="112" borderId="144" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="113" borderId="145" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="114" borderId="146" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="115" borderId="147" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="148" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="117" borderId="149" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="118" borderId="150" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="119" borderId="151" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="120" borderId="152" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="121" borderId="153" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="122" borderId="154" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="123" borderId="155" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="124" borderId="156" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="125" borderId="157" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="126" borderId="158" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="127" borderId="159" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="128" borderId="160" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="129" borderId="161" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="130" borderId="162" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="131" borderId="163" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="132" borderId="164" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="133" borderId="165" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="134" borderId="166" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="135" borderId="167" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="136" borderId="168" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="137" borderId="169" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="138" borderId="170" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="139" borderId="171" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="140" borderId="172" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="141" borderId="173" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="142" borderId="174" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="143" borderId="175" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="144" borderId="176" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="145" borderId="177" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="146" borderId="178" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="147" borderId="179" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="148" borderId="180" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="149" borderId="181" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="150" borderId="182" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="151" borderId="183" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="152" borderId="184" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="153" borderId="185" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="154" borderId="186" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="155" borderId="187" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="156" borderId="188" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="157" borderId="189" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="158" borderId="190" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="159" borderId="191" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="82" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" borderId="199" fillId="161" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="199" fillId="163" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="207" fillId="165" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="207" fillId="167" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="215" fillId="169" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="215" fillId="171" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="223" fillId="173" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="223" fillId="175" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="231" fillId="177" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="231" fillId="179" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="181" borderId="239" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="183" borderId="239" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6741,10 +6197,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -6779,7 +6235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -6814,7 +6270,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -6908,21 +6364,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -6939,7 +6395,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -6991,15 +6447,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:J62"/>
   <sheetViews>
     <sheetView topLeftCell="H16" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
@@ -7007,12 +6463,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="37.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="47.109375" collapsed="true"/>
-    <col min="7" max="7" style="23" width="9.109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="58.0" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" width="46.88671875" collapsed="true"/>
+    <col min="4" max="4" width="37.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.109375" style="23" collapsed="1"/>
+    <col min="8" max="8" width="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="46.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
@@ -7185,7 +6641,7 @@
       <c r="I22" s="50"/>
       <c r="J22" s="50"/>
     </row>
-    <row ht="15.6" r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="28"/>
       <c r="H23" s="56" t="s">
         <v>289</v>
@@ -7197,7 +6653,7 @@
         <v>539</v>
       </c>
     </row>
-    <row ht="15.6" r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="29"/>
       <c r="H24" s="250">
         <v>96501</v>
@@ -7207,7 +6663,7 @@
       </c>
       <c r="J24" s="55"/>
     </row>
-    <row ht="15.6" r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="58"/>
       <c r="H25" s="250"/>
       <c r="I25" s="70">
@@ -7215,7 +6671,7 @@
       </c>
       <c r="J25" s="55"/>
     </row>
-    <row ht="15.6" r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
       <c r="H26" s="250"/>
       <c r="I26" s="180">
@@ -7223,37 +6679,37 @@
       </c>
       <c r="J26" s="55"/>
     </row>
-    <row ht="15.6" r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="75"/>
       <c r="H27" s="250"/>
       <c r="I27" s="76"/>
       <c r="J27" s="55"/>
     </row>
-    <row ht="15.6" r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="75"/>
       <c r="H28" s="250"/>
       <c r="I28" s="76"/>
       <c r="J28" s="55"/>
     </row>
-    <row ht="15.6" r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="58"/>
       <c r="H29" s="250"/>
       <c r="I29" s="76"/>
       <c r="J29" s="55"/>
     </row>
-    <row ht="15.6" r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="16"/>
       <c r="H30" s="249"/>
       <c r="I30" s="55"/>
       <c r="J30" s="55"/>
     </row>
-    <row ht="15.6" r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="17"/>
       <c r="H31" s="249"/>
       <c r="I31" s="55"/>
       <c r="J31" s="55"/>
     </row>
-    <row ht="15.6" r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="18"/>
       <c r="H32" s="249"/>
       <c r="I32" s="55"/>
@@ -7404,16 +6860,16 @@
     <mergeCell ref="E38:E51"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink display="http://demo.guru99.com/v4/manager/addcustomerpage.php" r:id="rId1" ref="H7" xr:uid="{5475507B-EF53-4435-967A-8E1DB25565D1}"/>
+    <hyperlink ref="H7" r:id="rId1" display="http://demo.guru99.com/v4/manager/addcustomerpage.php" xr:uid="{5475507B-EF53-4435-967A-8E1DB25565D1}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -7421,11 +6877,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="87.88671875" collapsed="true"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="87.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -7981,15 +7437,15 @@
       <c r="I22" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -7997,11 +7453,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="98" width="133.5546875" collapsed="true"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="133.5546875" style="98" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -8582,14 +8038,14 @@
       <c r="A28" s="94"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:T15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B9"/>
@@ -8597,9 +8053,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="34.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -8796,15 +8252,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E9"/>
@@ -8812,9 +8268,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="34.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -8947,13 +8403,13 @@
       <c r="E9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:J23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -8961,9 +8417,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="34.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="47.44140625" collapsed="true"/>
+    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -9378,17 +8834,17 @@
       <c r="I23" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -9396,12 +8852,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="51.109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="55.5546875" collapsed="true"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="55.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -9446,7 +8902,7 @@
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="258" t="s">
+      <c r="G2" s="246" t="s">
         <v>491</v>
       </c>
     </row>
@@ -9621,34 +9077,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2" xr:uid="{A1042357-F7A5-452E-853D-7E0B1747F9AB}"/>
-    <hyperlink r:id="rId2" ref="E9" xr:uid="{93B52504-CADC-47D5-B084-8E8874572F05}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A1042357-F7A5-452E-853D-7E0B1747F9AB}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{93B52504-CADC-47D5-B084-8E8874572F05}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" workbookViewId="0">
+    <sheetView topLeftCell="J4" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="52.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="7" width="10.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="37.6640625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="33.5546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="2" max="2" width="52.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="37.6640625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -10066,7 +9522,7 @@
         <v>112</v>
       </c>
       <c r="N9" s="245" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="O9" s="245" t="s">
         <v>545</v>
@@ -10113,7 +9569,7 @@
         <v>112</v>
       </c>
       <c r="N10" s="205" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="O10" s="205" t="s">
         <v>545</v>
@@ -10160,7 +9616,7 @@
         <v>112</v>
       </c>
       <c r="N11" s="206" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="O11" s="206" t="s">
         <v>545</v>
@@ -10207,7 +9663,7 @@
         <v>112</v>
       </c>
       <c r="N12" s="207" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="O12" s="207" t="s">
         <v>545</v>
@@ -10254,7 +9710,7 @@
         <v>112</v>
       </c>
       <c r="N13" s="208" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="O13" s="208" t="s">
         <v>545</v>
@@ -10301,7 +9757,7 @@
         <v>112</v>
       </c>
       <c r="N14" s="209" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="O14" s="209" t="s">
         <v>545</v>
@@ -10348,7 +9804,7 @@
         <v>112</v>
       </c>
       <c r="N15" s="210" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O15" s="210" t="s">
         <v>545</v>
@@ -10395,7 +9851,7 @@
         <v>112</v>
       </c>
       <c r="N16" s="211" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O16" s="211" t="s">
         <v>545</v>
@@ -10439,13 +9895,13 @@
         <v>110</v>
       </c>
       <c r="M17" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="N17" s="247" t="s">
+        <v>336</v>
+      </c>
+      <c r="O17" s="247" t="s">
         <v>616</v>
-      </c>
-      <c r="N17" s="260" t="s">
-        <v>336</v>
-      </c>
-      <c r="O17" s="260" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -10486,13 +9942,13 @@
         <v>110</v>
       </c>
       <c r="M18" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="N18" s="248" t="s">
+        <v>336</v>
+      </c>
+      <c r="O18" s="248" t="s">
         <v>616</v>
-      </c>
-      <c r="N18" s="262" t="s">
-        <v>336</v>
-      </c>
-      <c r="O18" s="262" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -10537,7 +9993,7 @@
         <v>336</v>
       </c>
       <c r="O19" s="212" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -10584,7 +10040,7 @@
         <v>336</v>
       </c>
       <c r="O20" s="213" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -10631,7 +10087,7 @@
         <v>336</v>
       </c>
       <c r="O21" s="214" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -10723,7 +10179,7 @@
         <v>336</v>
       </c>
       <c r="O23" s="216" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -10768,7 +10224,7 @@
         <v>336</v>
       </c>
       <c r="O24" s="217" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -10815,7 +10271,7 @@
         <v>336</v>
       </c>
       <c r="O25" s="218" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -10907,7 +10363,7 @@
         <v>336</v>
       </c>
       <c r="O27" s="220" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -10954,7 +10410,7 @@
         <v>336</v>
       </c>
       <c r="O28" s="221" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -11001,7 +10457,7 @@
         <v>336</v>
       </c>
       <c r="O29" s="222" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -11093,7 +10549,7 @@
         <v>336</v>
       </c>
       <c r="O31" s="224" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -11140,7 +10596,7 @@
         <v>336</v>
       </c>
       <c r="O32" s="225" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -11187,7 +10643,7 @@
         <v>336</v>
       </c>
       <c r="O33" s="226" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -11279,7 +10735,7 @@
         <v>336</v>
       </c>
       <c r="O35" s="228" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -11326,7 +10782,7 @@
         <v>336</v>
       </c>
       <c r="O36" s="229" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -11467,7 +10923,7 @@
         <v>336</v>
       </c>
       <c r="O39" s="232" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -11512,7 +10968,7 @@
         <v>336</v>
       </c>
       <c r="O40" s="233" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -11559,7 +11015,7 @@
         <v>336</v>
       </c>
       <c r="O41" s="234" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -11698,7 +11154,7 @@
         <v>336</v>
       </c>
       <c r="O44" s="237" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -11745,7 +11201,7 @@
         <v>336</v>
       </c>
       <c r="O45" s="238" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -11792,7 +11248,7 @@
         <v>336</v>
       </c>
       <c r="O46" s="239" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -11839,7 +11295,7 @@
         <v>336</v>
       </c>
       <c r="O47" s="240" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
@@ -11886,7 +11342,7 @@
         <v>336</v>
       </c>
       <c r="O48" s="241" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -11934,7 +11390,7 @@
         <v>336</v>
       </c>
       <c r="O49" s="242" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -12006,7 +11462,7 @@
         <v>336</v>
       </c>
       <c r="O51" s="244" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -12054,82 +11510,82 @@
   </sheetData>
   <autoFilter ref="M1:M54" xr:uid="{2E414AA0-C410-4901-848C-351179CBD742}"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="K3" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink r:id="rId2" ref="K4" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink r:id="rId3" ref="K19" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink r:id="rId4" ref="K20" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink r:id="rId5" ref="K21" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink r:id="rId6" ref="K22" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink r:id="rId7" ref="K5" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink r:id="rId8" ref="K6" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink r:id="rId9" ref="K23" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink display="keya@test.com" r:id="rId10" ref="K7" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink r:id="rId11" ref="K24" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink r:id="rId12" ref="K25" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink r:id="rId13" ref="K8" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink r:id="rId14" ref="K26" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink r:id="rId15" ref="K9" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink r:id="rId16" ref="K27" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink r:id="rId17" ref="L13" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink r:id="rId18" ref="K28" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink r:id="rId19" ref="K29" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink r:id="rId20" ref="K30" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink r:id="rId21" ref="K17" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink r:id="rId22" ref="K31" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink r:id="rId23" ref="K32" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink r:id="rId24" ref="K33" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink r:id="rId25" ref="K34" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink r:id="rId26" ref="K18" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink r:id="rId27" ref="K35" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink r:id="rId28" ref="K36" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
-    <hyperlink r:id="rId29" ref="K37" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
-    <hyperlink r:id="rId30" ref="K38" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
-    <hyperlink r:id="rId31" ref="K10" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
-    <hyperlink r:id="rId32" ref="K39" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
-    <hyperlink r:id="rId33" ref="K40" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
-    <hyperlink r:id="rId34" ref="K41" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
-    <hyperlink r:id="rId35" ref="K42" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
-    <hyperlink r:id="rId36" ref="K43" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
-    <hyperlink r:id="rId37" ref="K11" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
-    <hyperlink r:id="rId38" ref="K12" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
-    <hyperlink display="roo@test.com" r:id="rId39" ref="K46" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
-    <hyperlink r:id="rId40" ref="K47" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
-    <hyperlink display="dar@test.com" r:id="rId41" ref="K48" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
-    <hyperlink r:id="rId42" ref="K14" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
-    <hyperlink r:id="rId43" ref="K50" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
-    <hyperlink r:id="rId44" ref="K13" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
-    <hyperlink r:id="rId45" ref="K15" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
-    <hyperlink r:id="rId46" ref="K16" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
-    <hyperlink display="kei@test.com" r:id="rId47" ref="K49" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
-    <hyperlink r:id="rId48" ref="K7" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
-    <hyperlink r:id="rId49" ref="K52" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
-    <hyperlink display="jos@guest.com" r:id="rId50" ref="K2" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="K19" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="K20" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="K21" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="K22" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="K5" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="K6" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="K23" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="K7" r:id="rId10" display="keya@test.com" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="K24" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="K25" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="K8" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="K26" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="K9" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="K27" r:id="rId16" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="L13" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="K28" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="K29" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="K30" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="K17" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="K31" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="K32" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="K33" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="K34" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="K18" r:id="rId26" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="K35" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="K36" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="K37" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="K38" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="K10" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="K39" r:id="rId32" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="K40" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="K41" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="K42" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="K43" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="K11" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="K12" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="K46" r:id="rId39" display="roo@test.com" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="K47" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="K48" r:id="rId41" display="dar@test.com" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="K14" r:id="rId42" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="K50" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="K13" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="K15" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="K16" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="K49" r:id="rId47" display="kei@test.com" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="K7" r:id="rId48" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="K52" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="K2" r:id="rId50" display="jos@guest.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId51"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="43.109375" collapsed="true"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="43.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -12412,7 +11868,7 @@
         <v>498</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -12571,7 +12027,7 @@
         <v>500</v>
       </c>
     </row>
-    <row ht="72" r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -12608,36 +12064,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I4" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink r:id="rId2" ref="I5" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink r:id="rId3" ref="I6" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink r:id="rId4" ref="I7" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink r:id="rId5" ref="I8" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink r:id="rId6" ref="I3" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink r:id="rId7" ref="I2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="I3" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="39.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="39.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -12770,7 +12226,7 @@
         <v>252</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>250</v>
@@ -12785,7 +12241,7 @@
         <v>252</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>250</v>
@@ -12800,7 +12256,7 @@
         <v>252</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>250</v>
@@ -12815,7 +12271,7 @@
         <v>252</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>250</v>
@@ -12830,7 +12286,7 @@
         <v>252</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>250</v>
@@ -12845,7 +12301,7 @@
         <v>252</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>250</v>
@@ -12860,7 +12316,7 @@
         <v>252</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>250</v>
@@ -12875,7 +12331,7 @@
         <v>252</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>250</v>
@@ -12970,7 +12426,7 @@
       </c>
       <c r="E22" s="49"/>
     </row>
-    <row ht="43.2" r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -12978,14 +12434,14 @@
         <v>261</v>
       </c>
       <c r="C23" s="1">
-        <v>10003459012</v>
+        <v>10003459054</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>255</v>
       </c>
       <c r="E23" s="49"/>
     </row>
-    <row ht="43.2" r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -13000,7 +12456,7 @@
       </c>
       <c r="E24" s="49"/>
     </row>
-    <row customHeight="1" ht="15" r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -13015,7 +12471,7 @@
       </c>
       <c r="E25" s="194"/>
     </row>
-    <row customHeight="1" ht="15" r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="103"/>
       <c r="B26" s="196" t="s">
         <v>449</v>
@@ -13028,7 +12484,7 @@
       </c>
       <c r="E26" s="195"/>
     </row>
-    <row customHeight="1" ht="15" r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="51"/>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
@@ -13036,18 +12492,18 @@
       <c r="E27" s="195"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
@@ -13055,14 +12511,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="40.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="52.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="34.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="30.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -13756,18 +13212,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
@@ -13775,9 +13231,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="62.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="36.5546875" collapsed="true"/>
+    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -13800,7 +13256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15.6" r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -13836,7 +13292,7 @@
         <v>537</v>
       </c>
     </row>
-    <row ht="15.6" r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -13998,7 +13454,7 @@
         <v>538</v>
       </c>
     </row>
-    <row ht="28.8" r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -14017,17 +13473,17 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -14035,10 +13491,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -14381,7 +13837,7 @@
         <v>355</v>
       </c>
     </row>
-    <row ht="72" r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -14410,14 +13866,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -14425,10 +13881,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="51.88671875" collapsed="true"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="51.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -14913,7 +14369,7 @@
       <c r="I20" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified updateNewAcctStatusInExcel and added delete method for editAcct
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/bin/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/bin/guru99/DataFiles/Guru99_testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5441AD-8745-4A45-A256-BEAF8AF0D3A3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC67D945-847B-4783-B639-0DD5115D3D49}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="622">
   <si>
     <t>testcaseID</t>
   </si>
@@ -1843,21 +1843,6 @@
     <t>45003459012</t>
   </si>
   <si>
-    <t>44553</t>
-  </si>
-  <si>
-    <t>44554</t>
-  </si>
-  <si>
-    <t>44555</t>
-  </si>
-  <si>
-    <t>44556</t>
-  </si>
-  <si>
-    <t>44557</t>
-  </si>
-  <si>
     <t>44558</t>
   </si>
   <si>
@@ -2126,6 +2111,41 @@
   </si>
   <si>
     <t>Pass - Customer could not be added !!</t>
+  </si>
+  <si>
+    <t>Pass - Customer deleted Successfully</t>
+  </si>
+  <si>
+    <t>Pass - You are not authorize to delete this customer!!</t>
+  </si>
+  <si>
+    <t>Pass - Customer could not be deleted!!. First delete all accounts of this customer then delete the customer</t>
+  </si>
+  <si>
+    <t>44680</t>
+  </si>
+  <si>
+    <t>44681</t>
+  </si>
+  <si>
+    <t>44682</t>
+  </si>
+  <si>
+    <t>44683</t>
+  </si>
+  <si>
+    <t>44684</t>
+  </si>
+  <si>
+    <t>Fail - org.openqa.selenium.TimeoutException: Expected condition failed: waiting for alert to be present (tried for 15 second(s) with 500 milliseconds interval)
+Build info: version: '3.12.0', revision: '7c6e0b3', time: '2018-05-08T15:15:08.936Z'
+System info: host: 'VINSCORPION', ip: '192.168.1.6', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '10.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.38.552522 (437e6fbedfa876..., userDataDir: C:\Users\vinay\AppData\Loca...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 67.0.3396.87, webStorageEnabled: true}
+Session ID: 664fd41720c3120226d9cdd2f3345dd8</t>
+  </si>
+  <si>
+    <t>Fail - Message mismatch..No Changes made to Account records</t>
   </si>
 </sst>
 </file>
@@ -2239,7 +2259,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="160">
+  <fills count="185">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3040,8 +3060,133 @@
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="192">
+  <borders count="217">
     <border>
       <left/>
       <right/>
@@ -5015,111 +5160,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -5129,6 +5169,486 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -5901,7 +6421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -6091,29 +6611,28 @@
     <xf numFmtId="0" fontId="0" fillId="90" borderId="121" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="91" borderId="122" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="92" borderId="123" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="93" borderId="124" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="94" borderId="125" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="95" borderId="126" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="96" borderId="127" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="97" borderId="128" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="98" borderId="129" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="99" borderId="130" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="100" borderId="131" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="101" borderId="132" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="102" borderId="133" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="103" borderId="134" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="104" borderId="135" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="105" borderId="136" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="106" borderId="137" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="107" borderId="138" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="108" borderId="139" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="140" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="140" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="140" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="133" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="133" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="140" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="133" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="102" borderId="134" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="103" borderId="135" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="104" borderId="136" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="105" borderId="137" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="106" borderId="138" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="107" borderId="139" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="108" borderId="140" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="109" borderId="141" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="110" borderId="142" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="111" borderId="143" xfId="0" applyFill="1" applyBorder="1"/>
@@ -6165,6 +6684,31 @@
     <xf numFmtId="0" fontId="0" fillId="157" borderId="189" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="158" borderId="190" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="159" borderId="191" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="160" borderId="192" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="161" borderId="193" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="162" borderId="194" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="163" borderId="195" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="164" borderId="196" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="165" borderId="197" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="166" borderId="198" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="167" borderId="199" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="168" borderId="200" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="169" borderId="201" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="170" borderId="202" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="171" borderId="203" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="172" borderId="204" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="173" borderId="205" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="174" borderId="206" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="175" borderId="207" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="176" borderId="208" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="177" borderId="209" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="178" borderId="210" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="179" borderId="211" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="180" borderId="212" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="181" borderId="213" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="182" borderId="214" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="183" borderId="215" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="184" borderId="216" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6650,12 +7194,12 @@
         <v>290</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="29"/>
-      <c r="H24" s="250">
+      <c r="H24" s="274">
         <v>96501</v>
       </c>
       <c r="I24" s="70">
@@ -6665,7 +7209,7 @@
     </row>
     <row r="25" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="58"/>
-      <c r="H25" s="250"/>
+      <c r="H25" s="274"/>
       <c r="I25" s="70">
         <v>44566</v>
       </c>
@@ -6673,63 +7217,63 @@
     </row>
     <row r="26" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
-      <c r="H26" s="250"/>
-      <c r="I26" s="180">
+      <c r="H26" s="274"/>
+      <c r="I26" s="175">
         <v>44604</v>
       </c>
       <c r="J26" s="55"/>
     </row>
     <row r="27" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="75"/>
-      <c r="H27" s="250"/>
+      <c r="H27" s="274"/>
       <c r="I27" s="76"/>
       <c r="J27" s="55"/>
     </row>
     <row r="28" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="75"/>
-      <c r="H28" s="250"/>
+      <c r="H28" s="274"/>
       <c r="I28" s="76"/>
       <c r="J28" s="55"/>
     </row>
     <row r="29" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="58"/>
-      <c r="H29" s="250"/>
+      <c r="H29" s="274"/>
       <c r="I29" s="76"/>
       <c r="J29" s="55"/>
     </row>
     <row r="30" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="16"/>
-      <c r="H30" s="249"/>
+      <c r="H30" s="273"/>
       <c r="I30" s="55"/>
       <c r="J30" s="55"/>
     </row>
     <row r="31" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="17"/>
-      <c r="H31" s="249"/>
+      <c r="H31" s="273"/>
       <c r="I31" s="55"/>
       <c r="J31" s="55"/>
     </row>
     <row r="32" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="18"/>
-      <c r="H32" s="249"/>
+      <c r="H32" s="273"/>
       <c r="I32" s="55"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="19"/>
-      <c r="H33" s="249"/>
+      <c r="H33" s="273"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="20"/>
-      <c r="H34" s="249"/>
+      <c r="H34" s="273"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="21"/>
-      <c r="H35" s="249"/>
+      <c r="H35" s="273"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
@@ -6741,95 +7285,95 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="31"/>
-      <c r="E38" s="251" t="s">
+      <c r="E38" s="275" t="s">
         <v>515</v>
       </c>
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="32"/>
-      <c r="E39" s="251"/>
+      <c r="E39" s="275"/>
       <c r="F39" s="132" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" s="33"/>
-      <c r="E40" s="251"/>
+      <c r="E40" s="275"/>
       <c r="F40" s="132" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="34"/>
-      <c r="E41" s="251"/>
+      <c r="E41" s="275"/>
       <c r="F41" s="132" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="35"/>
-      <c r="E42" s="251"/>
+      <c r="E42" s="275"/>
       <c r="F42" s="132" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="E43" s="251"/>
+      <c r="E43" s="275"/>
       <c r="F43" s="132" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="36"/>
-      <c r="E44" s="251"/>
+      <c r="E44" s="275"/>
       <c r="F44" s="132" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="37"/>
-      <c r="E45" s="251"/>
+      <c r="E45" s="275"/>
       <c r="F45" s="132" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="38"/>
-      <c r="E46" s="251"/>
+      <c r="E46" s="275"/>
       <c r="F46" s="132" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="39"/>
-      <c r="E47" s="251"/>
+      <c r="E47" s="275"/>
       <c r="F47" s="132" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="40"/>
-      <c r="E48" s="251"/>
+      <c r="E48" s="275"/>
       <c r="F48" s="132" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E49" s="251"/>
+      <c r="E49" s="275"/>
       <c r="F49" s="132" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E50" s="251"/>
+      <c r="E50" s="275"/>
       <c r="F50" s="132" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="41"/>
-      <c r="E51" s="251"/>
+      <c r="E51" s="275"/>
       <c r="F51" s="133" t="s">
         <v>251</v>
       </c>
@@ -8902,7 +9446,7 @@
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="246" t="s">
+      <c r="G2" s="269" t="s">
         <v>491</v>
       </c>
     </row>
@@ -9092,7 +9636,7 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="J4" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -9186,7 +9730,7 @@
         <v>7771232345</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>110</v>
@@ -9194,11 +9738,11 @@
       <c r="M2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="198" t="s">
-        <v>546</v>
-      </c>
-      <c r="O2" s="198" t="s">
-        <v>545</v>
+      <c r="N2" s="190" t="s">
+        <v>541</v>
+      </c>
+      <c r="O2" s="190" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -9233,7 +9777,7 @@
         <v>7778907689</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>110</v>
@@ -9241,11 +9785,11 @@
       <c r="M3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N3" s="199" t="s">
-        <v>587</v>
-      </c>
-      <c r="O3" s="199" t="s">
-        <v>545</v>
+      <c r="N3" s="191" t="s">
+        <v>582</v>
+      </c>
+      <c r="O3" s="191" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -9280,7 +9824,7 @@
         <v>7771237890</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>110</v>
@@ -9288,11 +9832,11 @@
       <c r="M4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N4" s="200" t="s">
-        <v>588</v>
-      </c>
-      <c r="O4" s="200" t="s">
-        <v>545</v>
+      <c r="N4" s="192" t="s">
+        <v>583</v>
+      </c>
+      <c r="O4" s="192" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -9327,7 +9871,7 @@
         <v>4447895432</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>110</v>
@@ -9335,11 +9879,11 @@
       <c r="M5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N5" s="201" t="s">
-        <v>589</v>
-      </c>
-      <c r="O5" s="201" t="s">
-        <v>545</v>
+      <c r="N5" s="193" t="s">
+        <v>584</v>
+      </c>
+      <c r="O5" s="193" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -9372,7 +9916,7 @@
         <v>7779081234</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>110</v>
@@ -9380,11 +9924,11 @@
       <c r="M6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N6" s="202" t="s">
-        <v>590</v>
-      </c>
-      <c r="O6" s="202" t="s">
-        <v>545</v>
+      <c r="N6" s="194" t="s">
+        <v>585</v>
+      </c>
+      <c r="O6" s="194" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -9419,7 +9963,7 @@
         <v>7771236789</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>110</v>
@@ -9427,11 +9971,11 @@
       <c r="M7" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N7" s="203" t="s">
-        <v>591</v>
-      </c>
-      <c r="O7" s="203" t="s">
-        <v>545</v>
+      <c r="N7" s="195" t="s">
+        <v>586</v>
+      </c>
+      <c r="O7" s="195" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -9466,7 +10010,7 @@
         <v>8786357718</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>110</v>
@@ -9474,11 +10018,11 @@
       <c r="M8" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N8" s="204" t="s">
-        <v>592</v>
-      </c>
-      <c r="O8" s="204" t="s">
-        <v>545</v>
+      <c r="N8" s="196" t="s">
+        <v>587</v>
+      </c>
+      <c r="O8" s="196" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -9513,7 +10057,7 @@
         <v>4417657812</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>110</v>
@@ -9521,11 +10065,11 @@
       <c r="M9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N9" s="245" t="s">
-        <v>614</v>
-      </c>
-      <c r="O9" s="245" t="s">
-        <v>545</v>
+      <c r="N9" s="237" t="s">
+        <v>609</v>
+      </c>
+      <c r="O9" s="237" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -9560,7 +10104,7 @@
         <v>5658901234</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>110</v>
@@ -9568,11 +10112,11 @@
       <c r="M10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N10" s="205" t="s">
-        <v>593</v>
-      </c>
-      <c r="O10" s="205" t="s">
-        <v>545</v>
+      <c r="N10" s="197" t="s">
+        <v>588</v>
+      </c>
+      <c r="O10" s="197" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -9607,7 +10151,7 @@
         <v>8806785435</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>110</v>
@@ -9615,11 +10159,11 @@
       <c r="M11" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N11" s="206" t="s">
-        <v>594</v>
-      </c>
-      <c r="O11" s="206" t="s">
-        <v>545</v>
+      <c r="N11" s="198" t="s">
+        <v>589</v>
+      </c>
+      <c r="O11" s="198" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -9654,7 +10198,7 @@
         <v>2227658912</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>110</v>
@@ -9662,11 +10206,11 @@
       <c r="M12" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N12" s="207" t="s">
-        <v>595</v>
-      </c>
-      <c r="O12" s="207" t="s">
-        <v>545</v>
+      <c r="N12" s="199" t="s">
+        <v>590</v>
+      </c>
+      <c r="O12" s="199" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -9701,7 +10245,7 @@
         <v>7776528901</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>177</v>
@@ -9709,11 +10253,11 @@
       <c r="M13" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N13" s="208" t="s">
-        <v>596</v>
-      </c>
-      <c r="O13" s="208" t="s">
-        <v>545</v>
+      <c r="N13" s="200" t="s">
+        <v>591</v>
+      </c>
+      <c r="O13" s="200" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -9748,7 +10292,7 @@
         <v>90165328917</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>110</v>
@@ -9756,11 +10300,11 @@
       <c r="M14" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N14" s="209" t="s">
-        <v>597</v>
-      </c>
-      <c r="O14" s="209" t="s">
-        <v>545</v>
+      <c r="N14" s="201" t="s">
+        <v>592</v>
+      </c>
+      <c r="O14" s="201" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -9795,7 +10339,7 @@
         <v>9992346781</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>178</v>
@@ -9803,11 +10347,11 @@
       <c r="M15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N15" s="210" t="s">
-        <v>598</v>
-      </c>
-      <c r="O15" s="210" t="s">
-        <v>545</v>
+      <c r="N15" s="202" t="s">
+        <v>593</v>
+      </c>
+      <c r="O15" s="202" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -9842,7 +10386,7 @@
         <v>2226189271</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>179</v>
@@ -9850,11 +10394,11 @@
       <c r="M16" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N16" s="211" t="s">
-        <v>599</v>
-      </c>
-      <c r="O16" s="211" t="s">
-        <v>545</v>
+      <c r="N16" s="203" t="s">
+        <v>594</v>
+      </c>
+      <c r="O16" s="203" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -9889,19 +10433,19 @@
         <v>5557789012</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>110</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="N17" s="247" t="s">
+        <v>610</v>
+      </c>
+      <c r="N17" s="238" t="s">
         <v>336</v>
       </c>
-      <c r="O17" s="247" t="s">
-        <v>616</v>
+      <c r="O17" s="238" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -9936,19 +10480,19 @@
         <v>1239872361</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>110</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="N18" s="248" t="s">
+        <v>610</v>
+      </c>
+      <c r="N18" s="239" t="s">
         <v>336</v>
       </c>
-      <c r="O18" s="248" t="s">
-        <v>616</v>
+      <c r="O18" s="239" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -9981,7 +10525,7 @@
         <v>9991237890</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>110</v>
@@ -9989,11 +10533,11 @@
       <c r="M19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N19" s="212" t="s">
+      <c r="N19" s="204" t="s">
         <v>336</v>
       </c>
-      <c r="O19" s="212" t="s">
-        <v>600</v>
+      <c r="O19" s="204" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -10028,7 +10572,7 @@
         <v>5556789087</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>110</v>
@@ -10036,11 +10580,11 @@
       <c r="M20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N20" s="213" t="s">
+      <c r="N20" s="205" t="s">
         <v>336</v>
       </c>
-      <c r="O20" s="213" t="s">
-        <v>601</v>
+      <c r="O20" s="205" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -10075,7 +10619,7 @@
         <v>5554567897</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>110</v>
@@ -10083,11 +10627,11 @@
       <c r="M21" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N21" s="214" t="s">
+      <c r="N21" s="206" t="s">
         <v>336</v>
       </c>
-      <c r="O21" s="214" t="s">
-        <v>602</v>
+      <c r="O21" s="206" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -10122,7 +10666,7 @@
         <v>4448960786</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>110</v>
@@ -10130,10 +10674,10 @@
       <c r="M22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N22" s="215" t="s">
+      <c r="N22" s="207" t="s">
         <v>336</v>
       </c>
-      <c r="O22" s="215" t="s">
+      <c r="O22" s="207" t="s">
         <v>354</v>
       </c>
     </row>
@@ -10167,7 +10711,7 @@
         <v>7776892313</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>110</v>
@@ -10175,11 +10719,11 @@
       <c r="M23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="N23" s="216" t="s">
+      <c r="N23" s="208" t="s">
         <v>336</v>
       </c>
-      <c r="O23" s="216" t="s">
-        <v>603</v>
+      <c r="O23" s="208" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -10212,7 +10756,7 @@
         <v>2227657890</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>110</v>
@@ -10220,11 +10764,11 @@
       <c r="M24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="N24" s="217" t="s">
+      <c r="N24" s="209" t="s">
         <v>336</v>
       </c>
-      <c r="O24" s="217" t="s">
-        <v>604</v>
+      <c r="O24" s="209" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -10259,7 +10803,7 @@
         <v>90167189172</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>110</v>
@@ -10267,11 +10811,11 @@
       <c r="M25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N25" s="218" t="s">
+      <c r="N25" s="210" t="s">
         <v>336</v>
       </c>
-      <c r="O25" s="218" t="s">
-        <v>601</v>
+      <c r="O25" s="210" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -10306,7 +10850,7 @@
         <v>4417678901</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>110</v>
@@ -10314,10 +10858,10 @@
       <c r="M26" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N26" s="219" t="s">
+      <c r="N26" s="211" t="s">
         <v>336</v>
       </c>
-      <c r="O26" s="219" t="s">
+      <c r="O26" s="211" t="s">
         <v>354</v>
       </c>
     </row>
@@ -10351,7 +10895,7 @@
         <v>9997863271</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>110</v>
@@ -10359,11 +10903,11 @@
       <c r="M27" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="N27" s="220" t="s">
+      <c r="N27" s="212" t="s">
         <v>336</v>
       </c>
-      <c r="O27" s="220" t="s">
-        <v>605</v>
+      <c r="O27" s="212" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -10398,7 +10942,7 @@
         <v>6557891271</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>110</v>
@@ -10406,11 +10950,11 @@
       <c r="M28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N28" s="221" t="s">
+      <c r="N28" s="213" t="s">
         <v>336</v>
       </c>
-      <c r="O28" s="221" t="s">
-        <v>601</v>
+      <c r="O28" s="213" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -10445,7 +10989,7 @@
         <v>7779874561</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>110</v>
@@ -10453,11 +10997,11 @@
       <c r="M29" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N29" s="222" t="s">
+      <c r="N29" s="214" t="s">
         <v>336</v>
       </c>
-      <c r="O29" s="222" t="s">
-        <v>602</v>
+      <c r="O29" s="214" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -10492,7 +11036,7 @@
         <v>7779084515</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>110</v>
@@ -10500,10 +11044,10 @@
       <c r="M30" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N30" s="223" t="s">
+      <c r="N30" s="215" t="s">
         <v>336</v>
       </c>
-      <c r="O30" s="223" t="s">
+      <c r="O30" s="215" t="s">
         <v>354</v>
       </c>
     </row>
@@ -10537,7 +11081,7 @@
         <v>1018237829</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>110</v>
@@ -10545,11 +11089,11 @@
       <c r="M31" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N31" s="224" t="s">
+      <c r="N31" s="216" t="s">
         <v>336</v>
       </c>
-      <c r="O31" s="224" t="s">
-        <v>606</v>
+      <c r="O31" s="216" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -10584,7 +11128,7 @@
         <v>1015677890</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>110</v>
@@ -10592,11 +11136,11 @@
       <c r="M32" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N32" s="225" t="s">
+      <c r="N32" s="217" t="s">
         <v>336</v>
       </c>
-      <c r="O32" s="225" t="s">
-        <v>601</v>
+      <c r="O32" s="217" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -10631,7 +11175,7 @@
         <v>1012237893</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>110</v>
@@ -10639,11 +11183,11 @@
       <c r="M33" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N33" s="226" t="s">
+      <c r="N33" s="218" t="s">
         <v>336</v>
       </c>
-      <c r="O33" s="226" t="s">
-        <v>602</v>
+      <c r="O33" s="218" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -10678,7 +11222,7 @@
         <v>1016738377</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>110</v>
@@ -10686,10 +11230,10 @@
       <c r="M34" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N34" s="227" t="s">
+      <c r="N34" s="219" t="s">
         <v>336</v>
       </c>
-      <c r="O34" s="227" t="s">
+      <c r="O34" s="219" t="s">
         <v>354</v>
       </c>
     </row>
@@ -10723,7 +11267,7 @@
         <v>4417728910</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>110</v>
@@ -10731,11 +11275,11 @@
       <c r="M35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="N35" s="228" t="s">
+      <c r="N35" s="220" t="s">
         <v>336</v>
       </c>
-      <c r="O35" s="228" t="s">
-        <v>607</v>
+      <c r="O35" s="220" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -10770,7 +11314,7 @@
         <v>5657811232</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>110</v>
@@ -10778,11 +11322,11 @@
       <c r="M36" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N36" s="229" t="s">
+      <c r="N36" s="221" t="s">
         <v>336</v>
       </c>
-      <c r="O36" s="229" t="s">
-        <v>601</v>
+      <c r="O36" s="221" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -10817,7 +11361,7 @@
         <v>6628725671</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>110</v>
@@ -10825,10 +11369,10 @@
       <c r="M37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N37" s="230" t="s">
+      <c r="N37" s="222" t="s">
         <v>336</v>
       </c>
-      <c r="O37" s="230" t="s">
+      <c r="O37" s="222" t="s">
         <v>353</v>
       </c>
     </row>
@@ -10864,7 +11408,7 @@
         <v>5529874561</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>110</v>
@@ -10872,10 +11416,10 @@
       <c r="M38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N38" s="231" t="s">
+      <c r="N38" s="223" t="s">
         <v>336</v>
       </c>
-      <c r="O38" s="231" t="s">
+      <c r="O38" s="223" t="s">
         <v>354</v>
       </c>
     </row>
@@ -10911,7 +11455,7 @@
         <v>9328982123</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>110</v>
@@ -10919,11 +11463,11 @@
       <c r="M39" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N39" s="232" t="s">
+      <c r="N39" s="224" t="s">
         <v>336</v>
       </c>
-      <c r="O39" s="232" t="s">
-        <v>608</v>
+      <c r="O39" s="224" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -10956,7 +11500,7 @@
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="2" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>110</v>
@@ -10964,11 +11508,11 @@
       <c r="M40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N40" s="233" t="s">
+      <c r="N40" s="225" t="s">
         <v>336</v>
       </c>
-      <c r="O40" s="233" t="s">
-        <v>609</v>
+      <c r="O40" s="225" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -11003,7 +11547,7 @@
         <v>90</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>110</v>
@@ -11011,11 +11555,11 @@
       <c r="M41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N41" s="234" t="s">
+      <c r="N41" s="226" t="s">
         <v>336</v>
       </c>
-      <c r="O41" s="234" t="s">
-        <v>601</v>
+      <c r="O41" s="226" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -11050,7 +11594,7 @@
         <v>238</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>110</v>
@@ -11058,10 +11602,10 @@
       <c r="M42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N42" s="235" t="s">
+      <c r="N42" s="227" t="s">
         <v>336</v>
       </c>
-      <c r="O42" s="235" t="s">
+      <c r="O42" s="227" t="s">
         <v>353</v>
       </c>
     </row>
@@ -11097,7 +11641,7 @@
         <v>248</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>110</v>
@@ -11105,10 +11649,10 @@
       <c r="M43" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N43" s="236" t="s">
+      <c r="N43" s="228" t="s">
         <v>336</v>
       </c>
-      <c r="O43" s="236" t="s">
+      <c r="O43" s="228" t="s">
         <v>354</v>
       </c>
     </row>
@@ -11150,11 +11694,11 @@
       <c r="M44" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N44" s="237" t="s">
+      <c r="N44" s="229" t="s">
         <v>336</v>
       </c>
-      <c r="O44" s="237" t="s">
-        <v>610</v>
+      <c r="O44" s="229" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -11197,11 +11741,11 @@
       <c r="M45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N45" s="238" t="s">
+      <c r="N45" s="230" t="s">
         <v>336</v>
       </c>
-      <c r="O45" s="238" t="s">
-        <v>601</v>
+      <c r="O45" s="230" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -11244,11 +11788,11 @@
       <c r="M46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N46" s="239" t="s">
+      <c r="N46" s="231" t="s">
         <v>336</v>
       </c>
-      <c r="O46" s="239" t="s">
-        <v>611</v>
+      <c r="O46" s="231" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -11291,11 +11835,11 @@
       <c r="M47" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N47" s="240" t="s">
+      <c r="N47" s="232" t="s">
         <v>336</v>
       </c>
-      <c r="O47" s="240" t="s">
-        <v>611</v>
+      <c r="O47" s="232" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
@@ -11338,11 +11882,11 @@
       <c r="M48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N48" s="241" t="s">
+      <c r="N48" s="233" t="s">
         <v>336</v>
       </c>
-      <c r="O48" s="241" t="s">
-        <v>611</v>
+      <c r="O48" s="233" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -11386,11 +11930,11 @@
       <c r="M49" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="N49" s="242" t="s">
+      <c r="N49" s="234" t="s">
         <v>336</v>
       </c>
-      <c r="O49" s="242" t="s">
-        <v>612</v>
+      <c r="O49" s="234" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -11425,16 +11969,16 @@
         <v>8783426621</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N50" s="243" t="s">
+      <c r="N50" s="235" t="s">
         <v>336</v>
       </c>
-      <c r="O50" s="243" t="s">
+      <c r="O50" s="235" t="s">
         <v>494</v>
       </c>
     </row>
@@ -11458,11 +12002,11 @@
       <c r="M51" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="N51" s="244" t="s">
+      <c r="N51" s="236" t="s">
         <v>336</v>
       </c>
-      <c r="O51" s="244" t="s">
-        <v>613</v>
+      <c r="O51" s="236" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -11495,7 +12039,7 @@
         <v>9996278123</v>
       </c>
       <c r="K52" s="100" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="L52" s="86" t="s">
         <v>110</v>
@@ -11569,7 +12113,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
-    <tabColor theme="9"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -11631,7 +12175,7 @@
         <v>266</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>274</v>
@@ -11649,7 +12193,7 @@
         <v>7771232345</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>283</v>
@@ -11666,7 +12210,7 @@
         <v>267</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>39</v>
@@ -11684,7 +12228,7 @@
         <v>7771232345</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>283</v>
@@ -11701,7 +12245,7 @@
         <v>268</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>39</v>
@@ -11719,7 +12263,7 @@
         <v>7771232345</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>283</v>
@@ -11736,7 +12280,7 @@
         <v>269</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>275</v>
@@ -11754,7 +12298,7 @@
         <v>7771232345</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>283</v>
@@ -11771,7 +12315,7 @@
         <v>270</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>276</v>
@@ -11789,7 +12333,7 @@
         <v>7778901237</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>283</v>
@@ -11806,7 +12350,7 @@
         <v>271</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>277</v>
@@ -11841,7 +12385,7 @@
         <v>282</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>277</v>
@@ -11876,7 +12420,7 @@
         <v>272</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -12080,12 +12624,12 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12121,12 +12665,14 @@
         <v>252</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>546</v>
+        <v>336</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="49"/>
+      <c r="E2" s="240" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -12136,12 +12682,14 @@
         <v>252</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>587</v>
+        <v>336</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E3" s="49"/>
+      <c r="E3" s="241" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -12151,12 +12699,14 @@
         <v>252</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>588</v>
+        <v>336</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="242" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -12166,12 +12716,14 @@
         <v>252</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>589</v>
+        <v>336</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="243" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -12181,12 +12733,14 @@
         <v>252</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>590</v>
+        <v>336</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E6" s="49"/>
+      <c r="E6" s="244" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -12196,12 +12750,14 @@
         <v>252</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>591</v>
+        <v>336</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="49"/>
+      <c r="E7" s="245" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -12211,12 +12767,14 @@
         <v>252</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>592</v>
+        <v>336</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E8" s="49"/>
+      <c r="E8" s="246" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -12226,12 +12784,14 @@
         <v>252</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>593</v>
+        <v>336</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E9" s="49"/>
+      <c r="E9" s="247" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -12241,12 +12801,14 @@
         <v>252</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>594</v>
+        <v>336</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E10" s="49"/>
+      <c r="E10" s="248" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -12256,12 +12818,14 @@
         <v>252</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>595</v>
+        <v>336</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E11" s="49"/>
+      <c r="E11" s="249" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -12271,12 +12835,14 @@
         <v>252</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>596</v>
+        <v>336</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E12" s="49"/>
+      <c r="E12" s="250" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -12286,12 +12852,14 @@
         <v>252</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>597</v>
+        <v>336</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E13" s="49"/>
+      <c r="E13" s="251" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -12301,12 +12869,14 @@
         <v>252</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>598</v>
+        <v>336</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E14" s="49"/>
+      <c r="E14" s="252" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -12316,12 +12886,14 @@
         <v>252</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>599</v>
+        <v>336</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E15" s="49"/>
+      <c r="E15" s="253" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -12331,12 +12903,14 @@
         <v>252</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>614</v>
+        <v>336</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E16" s="49"/>
+      <c r="E16" s="254" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -12349,7 +12923,9 @@
       <c r="D17" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E17" s="49"/>
+      <c r="E17" s="255" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -12364,7 +12940,9 @@
       <c r="D18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="49"/>
+      <c r="E18" s="256" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -12379,7 +12957,9 @@
       <c r="D19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="49"/>
+      <c r="E19" s="257" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -12394,7 +12974,9 @@
       <c r="D20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="49"/>
+      <c r="E20" s="258" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -12409,7 +12991,9 @@
       <c r="D21" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E21" s="49"/>
+      <c r="E21" s="259" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -12424,7 +13008,9 @@
       <c r="D22" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E22" s="49"/>
+      <c r="E22" s="260" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -12439,7 +13025,9 @@
       <c r="D23" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E23" s="49"/>
+      <c r="E23" s="261" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -12454,26 +13042,30 @@
       <c r="D24" s="52" t="s">
         <v>294</v>
       </c>
-      <c r="E24" s="49"/>
+      <c r="E24" s="262" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="197" t="s">
+      <c r="B25" s="189" t="s">
         <v>366</v>
       </c>
-      <c r="C25" s="192">
+      <c r="C25" s="185">
         <v>37672</v>
       </c>
-      <c r="D25" s="193" t="s">
+      <c r="D25" s="186" t="s">
         <v>255</v>
       </c>
-      <c r="E25" s="194"/>
+      <c r="E25" s="263" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="103"/>
-      <c r="B26" s="196" t="s">
+      <c r="B26" s="188" t="s">
         <v>449</v>
       </c>
       <c r="C26" s="103">
@@ -12482,14 +13074,14 @@
       <c r="D26" s="50" t="s">
         <v>285</v>
       </c>
-      <c r="E26" s="195"/>
+      <c r="E26" s="187"/>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="51"/>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
-      <c r="E27" s="195"/>
+      <c r="E27" s="187"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12506,7 +13098,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12566,10 +13158,10 @@
       <c r="F2" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G2" s="134" t="s">
-        <v>522</v>
-      </c>
-      <c r="H2" s="134" t="s">
+      <c r="G2" s="264" t="s">
+        <v>615</v>
+      </c>
+      <c r="H2" s="264" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12592,10 +13184,10 @@
       <c r="F3" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G3" s="135" t="s">
-        <v>523</v>
-      </c>
-      <c r="H3" s="135" t="s">
+      <c r="G3" s="265" t="s">
+        <v>616</v>
+      </c>
+      <c r="H3" s="265" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12618,10 +13210,10 @@
       <c r="F4" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G4" s="136" t="s">
-        <v>524</v>
-      </c>
-      <c r="H4" s="136" t="s">
+      <c r="G4" s="266" t="s">
+        <v>617</v>
+      </c>
+      <c r="H4" s="266" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12644,10 +13236,10 @@
       <c r="F5" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G5" s="137" t="s">
-        <v>525</v>
-      </c>
-      <c r="H5" s="137" t="s">
+      <c r="G5" s="267" t="s">
+        <v>618</v>
+      </c>
+      <c r="H5" s="267" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12670,10 +13262,10 @@
       <c r="F6" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G6" s="138" t="s">
-        <v>526</v>
-      </c>
-      <c r="H6" s="138" t="s">
+      <c r="G6" s="268" t="s">
+        <v>619</v>
+      </c>
+      <c r="H6" s="268" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12696,10 +13288,10 @@
       <c r="F7" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G7" s="139" t="s">
-        <v>527</v>
-      </c>
-      <c r="H7" s="139" t="s">
+      <c r="G7" s="134" t="s">
+        <v>522</v>
+      </c>
+      <c r="H7" s="134" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12720,10 +13312,10 @@
       <c r="F8" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G8" s="140" t="s">
-        <v>528</v>
-      </c>
-      <c r="H8" s="140" t="s">
+      <c r="G8" s="135" t="s">
+        <v>523</v>
+      </c>
+      <c r="H8" s="135" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12746,10 +13338,10 @@
       <c r="F9" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G9" s="141" t="s">
-        <v>529</v>
-      </c>
-      <c r="H9" s="141" t="s">
+      <c r="G9" s="136" t="s">
+        <v>524</v>
+      </c>
+      <c r="H9" s="136" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12772,10 +13364,10 @@
       <c r="F10" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G10" s="142" t="s">
-        <v>530</v>
-      </c>
-      <c r="H10" s="142" t="s">
+      <c r="G10" s="137" t="s">
+        <v>525</v>
+      </c>
+      <c r="H10" s="137" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12798,10 +13390,10 @@
       <c r="F11" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G11" s="143" t="s">
-        <v>531</v>
-      </c>
-      <c r="H11" s="143" t="s">
+      <c r="G11" s="138" t="s">
+        <v>526</v>
+      </c>
+      <c r="H11" s="138" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12824,10 +13416,10 @@
       <c r="F12" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G12" s="144" t="s">
-        <v>532</v>
-      </c>
-      <c r="H12" s="144" t="s">
+      <c r="G12" s="139" t="s">
+        <v>527</v>
+      </c>
+      <c r="H12" s="139" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12850,10 +13442,10 @@
       <c r="F13" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G13" s="145" t="s">
-        <v>533</v>
-      </c>
-      <c r="H13" s="145" t="s">
+      <c r="G13" s="140" t="s">
+        <v>528</v>
+      </c>
+      <c r="H13" s="140" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12876,10 +13468,10 @@
       <c r="F14" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G14" s="146" t="s">
-        <v>534</v>
-      </c>
-      <c r="H14" s="146" t="s">
+      <c r="G14" s="141" t="s">
+        <v>529</v>
+      </c>
+      <c r="H14" s="141" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12900,11 +13492,11 @@
       <c r="F15" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G15" s="147" t="s">
+      <c r="G15" s="142" t="s">
         <v>336</v>
       </c>
-      <c r="H15" s="147" t="s">
-        <v>535</v>
+      <c r="H15" s="142" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -12926,11 +13518,11 @@
       <c r="F16" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G16" s="148" t="s">
+      <c r="G16" s="143" t="s">
         <v>336</v>
       </c>
-      <c r="H16" s="148" t="s">
-        <v>535</v>
+      <c r="H16" s="143" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -12952,11 +13544,11 @@
       <c r="F17" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G17" s="149" t="s">
+      <c r="G17" s="144" t="s">
         <v>336</v>
       </c>
-      <c r="H17" s="149" t="s">
-        <v>535</v>
+      <c r="H17" s="144" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -12978,11 +13570,11 @@
       <c r="F18" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G18" s="150" t="s">
+      <c r="G18" s="145" t="s">
         <v>336</v>
       </c>
-      <c r="H18" s="150" t="s">
-        <v>535</v>
+      <c r="H18" s="145" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -13004,11 +13596,11 @@
       <c r="F19" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G19" s="151" t="s">
+      <c r="G19" s="146" t="s">
         <v>336</v>
       </c>
-      <c r="H19" s="151" t="s">
-        <v>535</v>
+      <c r="H19" s="146" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -13028,11 +13620,11 @@
       <c r="F20" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G20" s="152" t="s">
+      <c r="G20" s="147" t="s">
         <v>336</v>
       </c>
-      <c r="H20" s="152" t="s">
-        <v>536</v>
+      <c r="H20" s="147" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -13054,11 +13646,11 @@
       <c r="F21" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G21" s="153" t="s">
+      <c r="G21" s="148" t="s">
         <v>336</v>
       </c>
-      <c r="H21" s="153" t="s">
-        <v>536</v>
+      <c r="H21" s="148" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -13080,11 +13672,11 @@
       <c r="F22" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G22" s="154" t="s">
+      <c r="G22" s="149" t="s">
         <v>336</v>
       </c>
-      <c r="H22" s="154" t="s">
-        <v>536</v>
+      <c r="H22" s="149" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -13106,11 +13698,11 @@
       <c r="F23" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G23" s="155" t="s">
+      <c r="G23" s="150" t="s">
         <v>336</v>
       </c>
-      <c r="H23" s="155" t="s">
-        <v>536</v>
+      <c r="H23" s="150" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -13132,11 +13724,11 @@
       <c r="F24" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G24" s="156" t="s">
+      <c r="G24" s="151" t="s">
         <v>336</v>
       </c>
-      <c r="H24" s="156" t="s">
-        <v>536</v>
+      <c r="H24" s="151" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -13158,11 +13750,11 @@
       <c r="F25" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G25" s="157" t="s">
+      <c r="G25" s="152" t="s">
         <v>336</v>
       </c>
-      <c r="H25" s="157" t="s">
-        <v>536</v>
+      <c r="H25" s="152" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -13178,11 +13770,11 @@
       <c r="F26" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G26" s="158" t="s">
+      <c r="G26" s="153" t="s">
         <v>336</v>
       </c>
-      <c r="H26" s="158" t="s">
-        <v>535</v>
+      <c r="H26" s="153" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -13204,11 +13796,11 @@
       <c r="F27" s="86" t="s">
         <v>514</v>
       </c>
-      <c r="G27" s="159" t="s">
+      <c r="G27" s="154" t="s">
         <v>336</v>
       </c>
-      <c r="H27" s="159" t="s">
-        <v>535</v>
+      <c r="H27" s="154" t="s">
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -13225,8 +13817,8 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13263,15 +13855,17 @@
       <c r="B2" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="C2" s="55"/>
+      <c r="C2" s="55" t="s">
+        <v>336</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>312</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="F2" s="181" t="s">
-        <v>540</v>
+      <c r="F2" s="270" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -13281,15 +13875,17 @@
       <c r="B3" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C3" s="180"/>
+      <c r="C3" s="175" t="s">
+        <v>336</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>311</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="F3" s="191" t="s">
-        <v>537</v>
+      <c r="F3" s="271" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -13299,15 +13895,17 @@
       <c r="B4" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="70" t="s">
+        <v>336</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>311</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="F4" s="181" t="s">
-        <v>540</v>
+      <c r="F4" s="272" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -13317,15 +13915,17 @@
       <c r="B5" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C5" s="180"/>
+      <c r="C5" s="175" t="s">
+        <v>336</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>312</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="F5" s="182" t="s">
-        <v>537</v>
+      <c r="F5" s="176" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -13344,8 +13944,8 @@
       <c r="E6" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F6" s="183" t="s">
-        <v>538</v>
+      <c r="F6" s="177" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -13360,8 +13960,8 @@
       <c r="E7" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="F7" s="184" t="s">
-        <v>541</v>
+      <c r="F7" s="178" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -13378,8 +13978,8 @@
       <c r="E8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="185" t="s">
-        <v>542</v>
+      <c r="F8" s="179" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -13396,8 +13996,8 @@
       <c r="E9" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="186" t="s">
-        <v>542</v>
+      <c r="F9" s="180" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -13414,8 +14014,8 @@
       <c r="E10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="187" t="s">
-        <v>543</v>
+      <c r="F10" s="181" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -13432,8 +14032,8 @@
       <c r="E11" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F11" s="188" t="s">
-        <v>538</v>
+      <c r="F11" s="182" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -13450,8 +14050,8 @@
       <c r="E12" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F12" s="189" t="s">
-        <v>538</v>
+      <c r="F12" s="183" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -13468,8 +14068,8 @@
       <c r="E13" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F13" s="190" t="s">
-        <v>538</v>
+      <c r="F13" s="184" t="s">
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -13527,7 +14127,7 @@
       <c r="D2" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E2" s="160" t="s">
+      <c r="E2" s="155" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13544,7 +14144,7 @@
       <c r="D3" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E3" s="161" t="s">
+      <c r="E3" s="156" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13561,7 +14161,7 @@
       <c r="D4" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E4" s="162" t="s">
+      <c r="E4" s="157" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13578,7 +14178,7 @@
       <c r="D5" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E5" s="163" t="s">
+      <c r="E5" s="158" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13595,7 +14195,7 @@
       <c r="D6" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E6" s="164" t="s">
+      <c r="E6" s="159" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13612,7 +14212,7 @@
       <c r="D7" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E7" s="165" t="s">
+      <c r="E7" s="160" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13629,7 +14229,7 @@
       <c r="D8" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E8" s="166" t="s">
+      <c r="E8" s="161" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13646,7 +14246,7 @@
       <c r="D9" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E9" s="167" t="s">
+      <c r="E9" s="162" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13663,7 +14263,7 @@
       <c r="D10" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E10" s="168" t="s">
+      <c r="E10" s="163" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13680,7 +14280,7 @@
       <c r="D11" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E11" s="169" t="s">
+      <c r="E11" s="164" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13697,7 +14297,7 @@
       <c r="D12" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E12" s="170" t="s">
+      <c r="E12" s="165" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13714,7 +14314,7 @@
       <c r="D13" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E13" s="171" t="s">
+      <c r="E13" s="166" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13731,7 +14331,7 @@
       <c r="D14" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E14" s="172" t="s">
+      <c r="E14" s="167" t="s">
         <v>516</v>
       </c>
     </row>
@@ -13748,7 +14348,7 @@
       <c r="D15" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E15" s="173" t="s">
+      <c r="E15" s="168" t="s">
         <v>352</v>
       </c>
     </row>
@@ -13765,7 +14365,7 @@
       <c r="D16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="174" t="s">
+      <c r="E16" s="169" t="s">
         <v>353</v>
       </c>
     </row>
@@ -13782,7 +14382,7 @@
       <c r="D17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="175" t="s">
+      <c r="E17" s="170" t="s">
         <v>353</v>
       </c>
     </row>
@@ -13799,7 +14399,7 @@
       <c r="D18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="176" t="s">
+      <c r="E18" s="171" t="s">
         <v>354</v>
       </c>
     </row>
@@ -13816,7 +14416,7 @@
       <c r="D19" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E19" s="177" t="s">
+      <c r="E19" s="172" t="s">
         <v>355</v>
       </c>
     </row>
@@ -13833,7 +14433,7 @@
       <c r="D20" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E20" s="178" t="s">
+      <c r="E20" s="173" t="s">
         <v>355</v>
       </c>
     </row>
@@ -13850,7 +14450,7 @@
       <c r="D21" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E21" s="179" t="s">
+      <c r="E21" s="174" t="s">
         <v>355</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified user name and added new jars with exe files
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/bin/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/bin/guru99/DataFiles/Guru99_testdata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E6AE33-DE9E-440B-B9E7-C0633EE2E67C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D43455-9E0B-4820-8394-44E193062904}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -364,7 +364,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="647">
   <si>
     <t>testcaseID</t>
   </si>
@@ -2296,6 +2296,15 @@
   </si>
   <si>
     <t>payee bal</t>
+  </si>
+  <si>
+    <t>mngr142473</t>
+  </si>
+  <si>
+    <t>savings</t>
+  </si>
+  <si>
+    <t>Account number without any transactions</t>
   </si>
 </sst>
 </file>
@@ -3470,11 +3479,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="52"/>
       </patternFill>
     </fill>
@@ -3567,6 +3571,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
       </patternFill>
     </fill>
   </fills>
@@ -7697,7 +7706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="335">
+  <cellXfs count="334">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -7766,7 +7775,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -8048,7 +8056,8 @@
     <xf numFmtId="0" fontId="0" fillId="226" borderId="273" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="227" borderId="274" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="228" borderId="275" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="229" borderId="276" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="229" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="230" borderId="276" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8058,7 +8067,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="230" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8343,7 +8351,7 @@
   <dimension ref="B2:J62"/>
   <sheetViews>
     <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H24" sqref="H24:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8357,7 +8365,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="H2" s="238" t="s">
+      <c r="H2" s="237" t="s">
         <v>594</v>
       </c>
     </row>
@@ -8372,162 +8380,162 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="H6" s="234" t="s">
+      <c r="H6" s="233" t="s">
         <v>604</v>
       </c>
-      <c r="I6" s="234"/>
-      <c r="J6" s="234" t="s">
+      <c r="I6" s="233"/>
+      <c r="J6" s="233" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
-      <c r="H7" s="235" t="s">
+      <c r="H7" s="234" t="s">
         <v>490</v>
       </c>
-      <c r="I7" s="234" t="s">
+      <c r="I7" s="233" t="s">
         <v>286</v>
       </c>
-      <c r="J7" s="234" t="s">
+      <c r="J7" s="233" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
-      <c r="H8" s="236" t="s">
+      <c r="H8" s="235" t="s">
         <v>491</v>
       </c>
-      <c r="I8" s="234" t="s">
+      <c r="I8" s="233" t="s">
         <v>287</v>
       </c>
-      <c r="J8" s="234" t="s">
+      <c r="J8" s="233" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="24"/>
-      <c r="H9" s="236" t="s">
+      <c r="H9" s="235" t="s">
         <v>492</v>
       </c>
-      <c r="I9" s="234" t="s">
+      <c r="I9" s="233" t="s">
         <v>288</v>
       </c>
-      <c r="J9" s="234" t="s">
+      <c r="J9" s="233" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="13"/>
-      <c r="H10" s="234"/>
-      <c r="I10" s="237" t="s">
+      <c r="H10" s="233"/>
+      <c r="I10" s="236" t="s">
         <v>295</v>
       </c>
-      <c r="J10" s="234" t="s">
+      <c r="J10" s="233" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
-      <c r="H11" s="234" t="s">
+      <c r="H11" s="233" t="s">
         <v>493</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="237" t="s">
+      <c r="I11" s="233"/>
+      <c r="J11" s="236" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="25"/>
-      <c r="H12" s="234" t="s">
+      <c r="H12" s="233" t="s">
         <v>494</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="234" t="s">
+      <c r="I12" s="233"/>
+      <c r="J12" s="233" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="77"/>
-      <c r="H13" s="234" t="s">
+      <c r="B13" s="76"/>
+      <c r="H13" s="233" t="s">
         <v>495</v>
       </c>
-      <c r="I13" s="234"/>
-      <c r="J13" s="234" t="s">
+      <c r="I13" s="233"/>
+      <c r="J13" s="233" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="77"/>
-      <c r="H14" s="234" t="s">
+      <c r="B14" s="76"/>
+      <c r="H14" s="233" t="s">
         <v>496</v>
       </c>
-      <c r="I14" s="234"/>
-      <c r="J14" s="234" t="s">
+      <c r="I14" s="233"/>
+      <c r="J14" s="233" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="77"/>
-      <c r="H15" s="234" t="s">
+      <c r="B15" s="76"/>
+      <c r="H15" s="233" t="s">
         <v>497</v>
       </c>
-      <c r="I15" s="234"/>
-      <c r="J15" s="234" t="s">
+      <c r="I15" s="233"/>
+      <c r="J15" s="233" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="77"/>
-      <c r="H16" s="234" t="s">
+      <c r="B16" s="76"/>
+      <c r="H16" s="233" t="s">
         <v>498</v>
       </c>
-      <c r="I16" s="234"/>
-      <c r="J16" s="234" t="s">
+      <c r="I16" s="233"/>
+      <c r="J16" s="233" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="77"/>
-      <c r="H17" s="234" t="s">
+      <c r="B17" s="76"/>
+      <c r="H17" s="233" t="s">
         <v>499</v>
       </c>
-      <c r="I17" s="234"/>
-      <c r="J17" s="234" t="s">
+      <c r="I17" s="233"/>
+      <c r="J17" s="233" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="77"/>
-      <c r="H18" s="234" t="s">
+      <c r="B18" s="76"/>
+      <c r="H18" s="233" t="s">
         <v>500</v>
       </c>
-      <c r="I18" s="234"/>
-      <c r="J18" s="234" t="s">
+      <c r="I18" s="233"/>
+      <c r="J18" s="233" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="15"/>
-      <c r="H19" s="234" t="s">
+      <c r="H19" s="233" t="s">
         <v>501</v>
       </c>
-      <c r="I19" s="234"/>
-      <c r="J19" s="234" t="s">
+      <c r="I19" s="233"/>
+      <c r="J19" s="233" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="26"/>
-      <c r="H20" s="234" t="s">
+      <c r="H20" s="233" t="s">
         <v>502</v>
       </c>
-      <c r="I20" s="234"/>
-      <c r="J20" s="234" t="s">
+      <c r="I20" s="233"/>
+      <c r="J20" s="233" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="77"/>
+      <c r="B21" s="76"/>
       <c r="H21" s="50"/>
       <c r="I21" s="50"/>
       <c r="J21" s="50"/>
@@ -8550,48 +8558,54 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="29"/>
       <c r="H24" s="332">
-        <v>96501</v>
-      </c>
-      <c r="I24" s="62">
-        <v>44363</v>
-      </c>
-      <c r="J24" s="55"/>
+        <v>62422</v>
+      </c>
+      <c r="I24">
+        <v>45565</v>
+      </c>
+      <c r="J24" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="25" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="58"/>
       <c r="H25" s="332"/>
-      <c r="I25" s="62">
-        <v>44566</v>
-      </c>
-      <c r="J25" s="55"/>
+      <c r="I25">
+        <v>45566</v>
+      </c>
+      <c r="J25" s="55" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="26" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
       <c r="H26" s="332"/>
-      <c r="I26" s="142">
-        <v>44604</v>
-      </c>
-      <c r="J26" s="55"/>
+      <c r="I26" s="53">
+        <v>45567</v>
+      </c>
+      <c r="J26" s="55" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="27" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="63"/>
+      <c r="B27" s="62"/>
       <c r="H27" s="332"/>
-      <c r="I27" s="64"/>
+      <c r="I27" s="63"/>
       <c r="J27" s="55"/>
     </row>
     <row r="28" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="63"/>
+      <c r="B28" s="62"/>
       <c r="H28" s="332"/>
-      <c r="I28" s="64"/>
+      <c r="I28" s="63"/>
       <c r="J28" s="55"/>
     </row>
     <row r="29" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="58"/>
       <c r="H29" s="332"/>
-      <c r="I29" s="64"/>
+      <c r="I29" s="63"/>
       <c r="J29" s="55"/>
     </row>
     <row r="30" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -8646,88 +8660,88 @@
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="32"/>
       <c r="E39" s="333"/>
-      <c r="F39" s="103" t="s">
+      <c r="F39" s="102" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" s="33"/>
       <c r="E40" s="333"/>
-      <c r="F40" s="103" t="s">
+      <c r="F40" s="102" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="34"/>
       <c r="E41" s="333"/>
-      <c r="F41" s="103" t="s">
+      <c r="F41" s="102" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="35"/>
       <c r="E42" s="333"/>
-      <c r="F42" s="103" t="s">
+      <c r="F42" s="102" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E43" s="333"/>
-      <c r="F43" s="103" t="s">
+      <c r="F43" s="102" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="36"/>
       <c r="E44" s="333"/>
-      <c r="F44" s="103" t="s">
+      <c r="F44" s="102" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="37"/>
       <c r="E45" s="333"/>
-      <c r="F45" s="103" t="s">
+      <c r="F45" s="102" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="38"/>
       <c r="E46" s="333"/>
-      <c r="F46" s="103" t="s">
+      <c r="F46" s="102" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="39"/>
       <c r="E47" s="333"/>
-      <c r="F47" s="103" t="s">
+      <c r="F47" s="102" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="40"/>
       <c r="E48" s="333"/>
-      <c r="F48" s="103" t="s">
+      <c r="F48" s="102" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E49" s="333"/>
-      <c r="F49" s="103" t="s">
+      <c r="F49" s="102" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E50" s="333"/>
-      <c r="F50" s="103" t="s">
+      <c r="F50" s="102" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="41"/>
       <c r="E51" s="333"/>
-      <c r="F51" s="104" t="s">
+      <c r="F51" s="103" t="s">
         <v>251</v>
       </c>
     </row>
@@ -8772,7 +8786,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8818,7 +8832,7 @@
       <c r="E2" s="49" t="s">
         <v>606</v>
       </c>
-      <c r="F2" s="239" t="s">
+      <c r="F2" s="238" t="s">
         <v>349</v>
       </c>
     </row>
@@ -8838,7 +8852,7 @@
       <c r="E3" s="49" t="s">
         <v>607</v>
       </c>
-      <c r="F3" s="240" t="s">
+      <c r="F3" s="239" t="s">
         <v>349</v>
       </c>
     </row>
@@ -8856,7 +8870,7 @@
       <c r="E4" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="F4" s="241" t="s">
+      <c r="F4" s="240" t="s">
         <v>350</v>
       </c>
     </row>
@@ -8876,7 +8890,7 @@
       <c r="E5" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="F5" s="242" t="s">
+      <c r="F5" s="241" t="s">
         <v>351</v>
       </c>
     </row>
@@ -8896,7 +8910,7 @@
       <c r="E6" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="F6" s="243" t="s">
+      <c r="F6" s="242" t="s">
         <v>351</v>
       </c>
     </row>
@@ -8916,7 +8930,7 @@
       <c r="E7" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="F7" s="244" t="s">
+      <c r="F7" s="243" t="s">
         <v>352</v>
       </c>
     </row>
@@ -8936,7 +8950,7 @@
       <c r="E8" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="F8" s="245" t="s">
+      <c r="F8" s="244" t="s">
         <v>353</v>
       </c>
     </row>
@@ -8956,7 +8970,7 @@
       <c r="E9" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="F9" s="246" t="s">
+      <c r="F9" s="245" t="s">
         <v>353</v>
       </c>
     </row>
@@ -8988,7 +9002,7 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -9026,7 +9040,7 @@
       <c r="H1" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="264" t="s">
+      <c r="I1" s="263" t="s">
         <v>5</v>
       </c>
     </row>
@@ -9037,7 +9051,7 @@
       <c r="B2" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>335</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -9052,10 +9066,10 @@
       <c r="G2" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H2" s="259" t="s">
+      <c r="H2" s="258" t="s">
         <v>615</v>
       </c>
-      <c r="I2" s="272" t="s">
+      <c r="I2" s="271" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9081,10 +9095,10 @@
       <c r="G3" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H3" s="259" t="s">
+      <c r="H3" s="258" t="s">
         <v>616</v>
       </c>
-      <c r="I3" s="273" t="s">
+      <c r="I3" s="272" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9110,10 +9124,10 @@
       <c r="G4" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H4" s="259" t="s">
+      <c r="H4" s="258" t="s">
         <v>617</v>
       </c>
-      <c r="I4" s="274" t="s">
+      <c r="I4" s="273" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9121,10 +9135,10 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="65" t="s">
         <v>379</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="64" t="s">
         <v>335</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -9139,10 +9153,10 @@
       <c r="G5" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H5" s="260" t="s">
+      <c r="H5" s="259" t="s">
         <v>615</v>
       </c>
-      <c r="I5" s="275" t="s">
+      <c r="I5" s="274" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9150,10 +9164,10 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="65" t="s">
         <v>380</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="64" t="s">
         <v>335</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -9168,10 +9182,10 @@
       <c r="G6" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H6" s="260" t="s">
+      <c r="H6" s="259" t="s">
         <v>618</v>
       </c>
-      <c r="I6" s="276" t="s">
+      <c r="I6" s="275" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9179,10 +9193,10 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="65" t="s">
         <v>381</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="64" t="s">
         <v>335</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -9197,10 +9211,10 @@
       <c r="G7" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H7" s="260" t="s">
+      <c r="H7" s="259" t="s">
         <v>610</v>
       </c>
-      <c r="I7" s="277" t="s">
+      <c r="I7" s="276" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9208,10 +9222,10 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="65" t="s">
         <v>383</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="64" t="s">
         <v>335</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -9226,10 +9240,10 @@
       <c r="G8" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H8" s="260" t="s">
+      <c r="H8" s="259" t="s">
         <v>619</v>
       </c>
-      <c r="I8" s="278" t="s">
+      <c r="I8" s="277" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9237,13 +9251,13 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="65" t="s">
         <v>377</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D9" s="142" t="s">
+      <c r="D9" s="141" t="s">
         <v>335</v>
       </c>
       <c r="E9" s="1">
@@ -9253,10 +9267,10 @@
       <c r="G9" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="H9" s="260" t="s">
+      <c r="H9" s="259" t="s">
         <v>620</v>
       </c>
-      <c r="I9" s="279" t="s">
+      <c r="I9" s="278" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9280,10 +9294,10 @@
       <c r="G10" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="H10" s="261" t="s">
+      <c r="H10" s="260" t="s">
         <v>599</v>
       </c>
-      <c r="I10" s="280" t="s">
+      <c r="I10" s="279" t="s">
         <v>353</v>
       </c>
     </row>
@@ -9309,10 +9323,10 @@
       <c r="G11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H11" s="262" t="s">
+      <c r="H11" s="261" t="s">
         <v>599</v>
       </c>
-      <c r="I11" s="281" t="s">
+      <c r="I11" s="280" t="s">
         <v>353</v>
       </c>
     </row>
@@ -9338,10 +9352,10 @@
       <c r="G12" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="262" t="s">
+      <c r="H12" s="261" t="s">
         <v>599</v>
       </c>
-      <c r="I12" s="282" t="s">
+      <c r="I12" s="281" t="s">
         <v>353</v>
       </c>
     </row>
@@ -9367,10 +9381,10 @@
       <c r="G13" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H13" s="262" t="s">
+      <c r="H13" s="261" t="s">
         <v>599</v>
       </c>
-      <c r="I13" s="283" t="s">
+      <c r="I13" s="282" t="s">
         <v>353</v>
       </c>
     </row>
@@ -9396,10 +9410,10 @@
       <c r="G14" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="H14" s="262" t="s">
+      <c r="H14" s="261" t="s">
         <v>599</v>
       </c>
-      <c r="I14" s="284" t="s">
+      <c r="I14" s="283" t="s">
         <v>353</v>
       </c>
     </row>
@@ -9425,10 +9439,10 @@
       <c r="G15" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="H15" s="263" t="s">
+      <c r="H15" s="262" t="s">
         <v>599</v>
       </c>
-      <c r="I15" s="285" t="s">
+      <c r="I15" s="284" t="s">
         <v>353</v>
       </c>
     </row>
@@ -9436,7 +9450,7 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="65" t="s">
         <v>372</v>
       </c>
       <c r="C16" s="1">
@@ -9452,10 +9466,10 @@
       <c r="G16" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="H16" s="260" t="s">
+      <c r="H16" s="259" t="s">
         <v>599</v>
       </c>
-      <c r="I16" s="286" t="s">
+      <c r="I16" s="285" t="s">
         <v>621</v>
       </c>
     </row>
@@ -9463,7 +9477,7 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>373</v>
       </c>
       <c r="C17" s="1">
@@ -9481,10 +9495,10 @@
       <c r="G17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H17" s="260" t="s">
+      <c r="H17" s="259" t="s">
         <v>599</v>
       </c>
-      <c r="I17" s="287" t="s">
+      <c r="I17" s="286" t="s">
         <v>621</v>
       </c>
     </row>
@@ -9492,7 +9506,7 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="65" t="s">
         <v>374</v>
       </c>
       <c r="C18" s="1">
@@ -9510,10 +9524,10 @@
       <c r="G18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="260" t="s">
+      <c r="H18" s="259" t="s">
         <v>599</v>
       </c>
-      <c r="I18" s="291" t="s">
+      <c r="I18" s="290" t="s">
         <v>622</v>
       </c>
     </row>
@@ -9521,7 +9535,7 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="65" t="s">
         <v>375</v>
       </c>
       <c r="C19" s="1">
@@ -9539,10 +9553,10 @@
       <c r="G19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="260" t="s">
+      <c r="H19" s="259" t="s">
         <v>599</v>
       </c>
-      <c r="I19" s="288" t="s">
+      <c r="I19" s="287" t="s">
         <v>621</v>
       </c>
     </row>
@@ -9550,7 +9564,7 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="65" t="s">
         <v>385</v>
       </c>
       <c r="C20" s="1"/>
@@ -9560,10 +9574,10 @@
       <c r="G20" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="H20" s="260" t="s">
+      <c r="H20" s="259" t="s">
         <v>599</v>
       </c>
-      <c r="I20" s="289" t="s">
+      <c r="I20" s="288" t="s">
         <v>353</v>
       </c>
     </row>
@@ -9571,7 +9585,7 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="65" t="s">
         <v>394</v>
       </c>
       <c r="C21" s="1">
@@ -9589,19 +9603,19 @@
       <c r="G21" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="H21" s="260" t="s">
+      <c r="H21" s="259" t="s">
         <v>599</v>
       </c>
-      <c r="I21" s="290" t="s">
+      <c r="I21" s="289" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="65" t="s">
         <v>395</v>
       </c>
-      <c r="C23" s="67">
+      <c r="C23" s="66">
         <v>39978</v>
       </c>
       <c r="D23" s="1">
@@ -9630,7 +9644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -9640,7 +9654,7 @@
     <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="38.88671875" style="71" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="38.88671875" style="70" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -9662,7 +9676,7 @@
       <c r="F1" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="68" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -9676,10 +9690,10 @@
       <c r="B2" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="71">
         <v>45017</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="71">
         <v>45024</v>
       </c>
       <c r="E2" s="1">
@@ -9688,10 +9702,10 @@
       <c r="F2" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G2" s="293" t="s">
+      <c r="G2" s="292" t="s">
         <v>426</v>
       </c>
-      <c r="H2" s="304" t="s">
+      <c r="H2" s="302" t="s">
         <v>635</v>
       </c>
     </row>
@@ -9702,10 +9716,10 @@
       <c r="B3" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C3" s="72">
+      <c r="C3" s="71">
         <v>45018</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="71">
         <v>45023</v>
       </c>
       <c r="E3" s="1">
@@ -9714,10 +9728,10 @@
       <c r="F3" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G3" s="293" t="s">
+      <c r="G3" s="292" t="s">
         <v>426</v>
       </c>
-      <c r="H3" s="305" t="s">
+      <c r="H3" s="303" t="s">
         <v>635</v>
       </c>
     </row>
@@ -9725,13 +9739,13 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="65" t="s">
         <v>379</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="71">
         <v>45019</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="71">
         <v>45022</v>
       </c>
       <c r="E4" s="1">
@@ -9740,10 +9754,10 @@
       <c r="F4" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G4" s="70" t="s">
+      <c r="G4" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="H4" s="306" t="s">
+      <c r="H4" s="304" t="s">
         <v>635</v>
       </c>
     </row>
@@ -9751,13 +9765,13 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="65" t="s">
         <v>380</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="71">
         <v>45020</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="71">
         <v>45021</v>
       </c>
       <c r="E5" s="1">
@@ -9766,10 +9780,10 @@
       <c r="F5" s="1">
         <v>908</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="H5" s="307" t="s">
+      <c r="H5" s="305" t="s">
         <v>635</v>
       </c>
     </row>
@@ -9777,13 +9791,13 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="65" t="s">
         <v>381</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="71">
         <v>45021</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="71">
         <v>45020</v>
       </c>
       <c r="E6" s="1">
@@ -9792,10 +9806,10 @@
       <c r="F6" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="H6" s="308" t="s">
+      <c r="H6" s="306" t="s">
         <v>635</v>
       </c>
     </row>
@@ -9803,13 +9817,13 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="65" t="s">
         <v>427</v>
       </c>
-      <c r="C7" s="72">
+      <c r="C7" s="71">
         <v>45022</v>
       </c>
-      <c r="D7" s="72">
+      <c r="D7" s="71">
         <v>45019</v>
       </c>
       <c r="E7" s="1">
@@ -9818,10 +9832,10 @@
       <c r="F7" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="G7" s="70" t="s">
+      <c r="G7" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="H7" s="309" t="s">
+      <c r="H7" s="307" t="s">
         <v>635</v>
       </c>
     </row>
@@ -9829,13 +9843,13 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="65" t="s">
         <v>625</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C8" s="71">
         <v>45023</v>
       </c>
-      <c r="D8" s="72">
+      <c r="D8" s="71">
         <v>45018</v>
       </c>
       <c r="E8" s="1">
@@ -9844,10 +9858,10 @@
       <c r="F8" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="G8" s="70" t="s">
+      <c r="G8" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="H8" s="310" t="s">
+      <c r="H8" s="308" t="s">
         <v>635</v>
       </c>
     </row>
@@ -9855,13 +9869,13 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="65" t="s">
         <v>424</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="71">
         <v>45024</v>
       </c>
-      <c r="D9" s="72">
+      <c r="D9" s="71">
         <v>45017</v>
       </c>
       <c r="E9" s="1">
@@ -9870,10 +9884,10 @@
       <c r="F9" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G9" s="70" t="s">
+      <c r="G9" s="69" t="s">
         <v>425</v>
       </c>
-      <c r="H9" s="311" t="s">
+      <c r="H9" s="309" t="s">
         <v>636</v>
       </c>
     </row>
@@ -9896,10 +9910,10 @@
       <c r="F10" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="G10" s="70" t="s">
+      <c r="G10" s="69" t="s">
         <v>400</v>
       </c>
-      <c r="H10" s="312" t="s">
+      <c r="H10" s="310" t="s">
         <v>637</v>
       </c>
     </row>
@@ -9921,7 +9935,7 @@
       <c r="G11" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="H11" s="313" t="s">
+      <c r="H11" s="311" t="s">
         <v>638</v>
       </c>
     </row>
@@ -9945,7 +9959,7 @@
       <c r="G12" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="314" t="s">
+      <c r="H12" s="312" t="s">
         <v>638</v>
       </c>
     </row>
@@ -9969,7 +9983,7 @@
       <c r="G13" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H13" s="315" t="s">
+      <c r="H13" s="313" t="s">
         <v>638</v>
       </c>
     </row>
@@ -9993,7 +10007,7 @@
       <c r="G14" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="316" t="s">
+      <c r="H14" s="314" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10012,10 +10026,10 @@
       <c r="F15" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G15" s="70" t="s">
+      <c r="G15" s="69" t="s">
         <v>418</v>
       </c>
-      <c r="H15" s="317" t="s">
+      <c r="H15" s="315" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10034,10 +10048,10 @@
       <c r="F16" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G16" s="70" t="s">
+      <c r="G16" s="69" t="s">
         <v>421</v>
       </c>
-      <c r="H16" s="318" t="s">
+      <c r="H16" s="316" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10059,7 +10073,7 @@
       <c r="G17" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H17" s="319" t="s">
+      <c r="H17" s="317" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10083,7 +10097,7 @@
       <c r="G18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="320" t="s">
+      <c r="H18" s="318" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10107,7 +10121,7 @@
       <c r="G19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="321" t="s">
+      <c r="H19" s="319" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10131,7 +10145,7 @@
       <c r="G20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H20" s="322" t="s">
+      <c r="H20" s="320" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10150,10 +10164,10 @@
       <c r="F21" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G21" s="70" t="s">
+      <c r="G21" s="69" t="s">
         <v>418</v>
       </c>
-      <c r="H21" s="323" t="s">
+      <c r="H21" s="321" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10172,10 +10186,10 @@
       <c r="F22" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G22" s="70" t="s">
+      <c r="G22" s="69" t="s">
         <v>421</v>
       </c>
-      <c r="H22" s="324" t="s">
+      <c r="H22" s="322" t="s">
         <v>638</v>
       </c>
     </row>
@@ -10183,7 +10197,7 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="65" t="s">
         <v>372</v>
       </c>
       <c r="C23" s="1">
@@ -10196,10 +10210,10 @@
       <c r="F23" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G23" s="70" t="s">
+      <c r="G23" s="69" t="s">
         <v>376</v>
       </c>
-      <c r="H23" s="325" t="s">
+      <c r="H23" s="323" t="s">
         <v>639</v>
       </c>
     </row>
@@ -10207,7 +10221,7 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="65" t="s">
         <v>373</v>
       </c>
       <c r="C24" s="1">
@@ -10222,10 +10236,10 @@
       <c r="F24" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G24" s="70" t="s">
+      <c r="G24" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="H24" s="326" t="s">
+      <c r="H24" s="324" t="s">
         <v>351</v>
       </c>
     </row>
@@ -10233,7 +10247,7 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="65" t="s">
         <v>374</v>
       </c>
       <c r="C25" s="1">
@@ -10248,10 +10262,10 @@
       <c r="F25" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G25" s="70" t="s">
+      <c r="G25" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="327" t="s">
+      <c r="H25" s="325" t="s">
         <v>351</v>
       </c>
     </row>
@@ -10259,7 +10273,7 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="65" t="s">
         <v>375</v>
       </c>
       <c r="C26" s="1">
@@ -10274,10 +10288,10 @@
       <c r="F26" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G26" s="70" t="s">
+      <c r="G26" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="H26" s="328" t="s">
+      <c r="H26" s="326" t="s">
         <v>352</v>
       </c>
     </row>
@@ -10285,7 +10299,7 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="65" t="s">
         <v>377</v>
       </c>
       <c r="C27" s="1">
@@ -10298,10 +10312,10 @@
         <v>10</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="70" t="s">
+      <c r="G27" s="69" t="s">
         <v>378</v>
       </c>
-      <c r="H27" s="329" t="s">
+      <c r="H27" s="327" t="s">
         <v>640</v>
       </c>
     </row>
@@ -10309,25 +10323,25 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="65" t="s">
         <v>414</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="70" t="s">
+      <c r="G28" s="69" t="s">
         <v>430</v>
       </c>
-      <c r="H28" s="330" t="s">
+      <c r="H28" s="328" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G29" s="292"/>
+      <c r="G29" s="291"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="294"/>
+      <c r="B33" s="293"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10337,16 +10351,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -10401,7 +10415,9 @@
         <v>323</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" t="s">
+        <v>324</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -10472,12 +10488,25 @@
         <v>343</v>
       </c>
       <c r="C9" s="1">
-        <v>1234589087</v>
+        <v>12345890871</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>333</v>
       </c>
       <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="65">
+        <v>9</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>646</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10676,7 +10705,7 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>458</v>
       </c>
       <c r="C10" s="1"/>
@@ -10693,7 +10722,7 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="65" t="s">
         <v>459</v>
       </c>
       <c r="C11" s="1"/>
@@ -10710,7 +10739,7 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="65" t="s">
         <v>460</v>
       </c>
       <c r="C12" s="1"/>
@@ -10727,7 +10756,7 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="65" t="s">
         <v>461</v>
       </c>
       <c r="C13" s="1"/>
@@ -10744,7 +10773,7 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C14" s="1"/>
@@ -10761,7 +10790,7 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="65" t="s">
         <v>466</v>
       </c>
       <c r="C15" s="1"/>
@@ -10778,7 +10807,7 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="65" t="s">
         <v>467</v>
       </c>
       <c r="C16" s="1"/>
@@ -10795,7 +10824,7 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>468</v>
       </c>
       <c r="C17" s="1"/>
@@ -10812,7 +10841,7 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="65" t="s">
         <v>470</v>
       </c>
       <c r="C18" s="1"/>
@@ -10829,7 +10858,7 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="65" t="s">
         <v>471</v>
       </c>
       <c r="C19" s="1"/>
@@ -10846,7 +10875,7 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="65" t="s">
         <v>472</v>
       </c>
       <c r="C20" s="1"/>
@@ -10863,7 +10892,7 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="65" t="s">
         <v>473</v>
       </c>
       <c r="C21" s="1"/>
@@ -10880,7 +10909,7 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="65" t="s">
         <v>474</v>
       </c>
       <c r="C22" s="1"/>
@@ -10897,7 +10926,7 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="65" t="s">
         <v>475</v>
       </c>
       <c r="C23" s="1"/>
@@ -10950,16 +10979,16 @@
       </c>
     </row>
     <row r="3" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F3" s="72">
+      <c r="F3" s="71">
         <v>45017</v>
       </c>
-      <c r="G3" s="72">
+      <c r="G3" s="71">
         <v>45024</v>
       </c>
-      <c r="H3" s="334">
+      <c r="H3" s="329">
         <v>980</v>
       </c>
-      <c r="I3" s="334">
+      <c r="I3" s="329">
         <v>510</v>
       </c>
       <c r="J3" s="1">
@@ -10975,16 +11004,16 @@
       </c>
     </row>
     <row r="4" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F4" s="72">
+      <c r="F4" s="71">
         <v>45018</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G4" s="71">
         <v>45023</v>
       </c>
-      <c r="H4" s="334">
+      <c r="H4" s="329">
         <v>480</v>
       </c>
-      <c r="I4" s="334">
+      <c r="I4" s="329">
         <v>510</v>
       </c>
       <c r="J4" s="1">
@@ -11000,16 +11029,16 @@
       </c>
     </row>
     <row r="5" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F5" s="72">
+      <c r="F5" s="71">
         <v>45019</v>
       </c>
-      <c r="G5" s="72">
+      <c r="G5" s="71">
         <v>45022</v>
       </c>
-      <c r="H5" s="334">
+      <c r="H5" s="329">
         <v>5979</v>
       </c>
-      <c r="I5" s="334">
+      <c r="I5" s="329">
         <v>1329</v>
       </c>
       <c r="J5" s="1">
@@ -11025,16 +11054,16 @@
       </c>
     </row>
     <row r="6" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F6" s="72">
+      <c r="F6" s="71">
         <v>45020</v>
       </c>
-      <c r="G6" s="72">
+      <c r="G6" s="71">
         <v>45021</v>
       </c>
-      <c r="H6" s="334">
+      <c r="H6" s="329">
         <v>4579</v>
       </c>
-      <c r="I6" s="334">
+      <c r="I6" s="329">
         <v>1139</v>
       </c>
       <c r="J6" s="1">
@@ -11050,16 +11079,16 @@
       </c>
     </row>
     <row r="7" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F7" s="72">
+      <c r="F7" s="71">
         <v>45021</v>
       </c>
-      <c r="G7" s="72">
+      <c r="G7" s="71">
         <v>45020</v>
       </c>
-      <c r="H7" s="334">
+      <c r="H7" s="329">
         <v>1189</v>
       </c>
-      <c r="I7" s="334"/>
+      <c r="I7" s="329"/>
       <c r="J7" s="1">
         <v>50</v>
       </c>
@@ -11073,16 +11102,16 @@
       </c>
     </row>
     <row r="8" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F8" s="72">
+      <c r="F8" s="71">
         <v>45022</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="71">
         <v>45019</v>
       </c>
-      <c r="H8" s="334">
+      <c r="H8" s="329">
         <v>1389</v>
       </c>
-      <c r="I8" s="334"/>
+      <c r="I8" s="329"/>
       <c r="J8" s="1">
         <v>60</v>
       </c>
@@ -11096,16 +11125,16 @@
       </c>
     </row>
     <row r="9" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F9" s="72">
+      <c r="F9" s="71">
         <v>45023</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="71">
         <v>45018</v>
       </c>
-      <c r="H9" s="334">
+      <c r="H9" s="329">
         <v>580</v>
       </c>
-      <c r="I9" s="334"/>
+      <c r="I9" s="329"/>
       <c r="J9" s="1">
         <v>70</v>
       </c>
@@ -11119,16 +11148,16 @@
       </c>
     </row>
     <row r="10" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F10" s="72">
+      <c r="F10" s="71">
         <v>45024</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="71">
         <v>45017</v>
       </c>
-      <c r="H10" s="334">
+      <c r="H10" s="329">
         <v>510</v>
       </c>
-      <c r="I10" s="334"/>
+      <c r="I10" s="329"/>
       <c r="J10" s="1">
         <v>99999999</v>
       </c>
@@ -11149,12 +11178,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor theme="9"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11201,7 +11230,7 @@
         <v>478</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>476</v>
+        <v>644</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>477</v>
@@ -11209,7 +11238,7 @@
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="303" t="s">
+      <c r="G2" s="330" t="s">
         <v>480</v>
       </c>
     </row>
@@ -11232,7 +11261,7 @@
       <c r="F3" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="79" t="s">
         <v>481</v>
       </c>
     </row>
@@ -11255,7 +11284,7 @@
       <c r="F4" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="G4" s="81" t="s">
+      <c r="G4" s="80" t="s">
         <v>481</v>
       </c>
     </row>
@@ -11278,7 +11307,7 @@
       <c r="F5" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="81" t="s">
         <v>481</v>
       </c>
     </row>
@@ -11299,7 +11328,7 @@
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="82" t="s">
         <v>482</v>
       </c>
     </row>
@@ -11320,7 +11349,7 @@
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="84" t="s">
+      <c r="G7" s="83" t="s">
         <v>483</v>
       </c>
     </row>
@@ -11339,7 +11368,7 @@
       <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="84" t="s">
         <v>484</v>
       </c>
     </row>
@@ -11354,7 +11383,7 @@
         <v>478</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>476</v>
+        <v>644</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>477</v>
@@ -11362,25 +11391,25 @@
       <c r="F9" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="85" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="79"/>
+      <c r="C10" s="78"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="79"/>
+      <c r="C11" s="78"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="79"/>
+      <c r="C12" s="78"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="79"/>
+      <c r="C13" s="78"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11501,10 +11530,10 @@
       <c r="M2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="148" t="s">
+      <c r="N2" s="147" t="s">
         <v>520</v>
       </c>
-      <c r="O2" s="148" t="s">
+      <c r="O2" s="147" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11548,10 +11577,10 @@
       <c r="M3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N3" s="149" t="s">
+      <c r="N3" s="148" t="s">
         <v>561</v>
       </c>
-      <c r="O3" s="149" t="s">
+      <c r="O3" s="148" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11595,10 +11624,10 @@
       <c r="M4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="149" t="s">
         <v>562</v>
       </c>
-      <c r="O4" s="150" t="s">
+      <c r="O4" s="149" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11642,10 +11671,10 @@
       <c r="M5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N5" s="151" t="s">
+      <c r="N5" s="150" t="s">
         <v>563</v>
       </c>
-      <c r="O5" s="151" t="s">
+      <c r="O5" s="150" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11687,10 +11716,10 @@
       <c r="M6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N6" s="152" t="s">
+      <c r="N6" s="151" t="s">
         <v>564</v>
       </c>
-      <c r="O6" s="152" t="s">
+      <c r="O6" s="151" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11734,10 +11763,10 @@
       <c r="M7" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N7" s="153" t="s">
+      <c r="N7" s="152" t="s">
         <v>565</v>
       </c>
-      <c r="O7" s="153" t="s">
+      <c r="O7" s="152" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11781,10 +11810,10 @@
       <c r="M8" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N8" s="154" t="s">
+      <c r="N8" s="153" t="s">
         <v>566</v>
       </c>
-      <c r="O8" s="154" t="s">
+      <c r="O8" s="153" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11828,10 +11857,10 @@
       <c r="M9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N9" s="195" t="s">
+      <c r="N9" s="194" t="s">
         <v>588</v>
       </c>
-      <c r="O9" s="195" t="s">
+      <c r="O9" s="194" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11875,10 +11904,10 @@
       <c r="M10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N10" s="155" t="s">
+      <c r="N10" s="154" t="s">
         <v>567</v>
       </c>
-      <c r="O10" s="155" t="s">
+      <c r="O10" s="154" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11922,10 +11951,10 @@
       <c r="M11" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N11" s="156" t="s">
+      <c r="N11" s="155" t="s">
         <v>568</v>
       </c>
-      <c r="O11" s="156" t="s">
+      <c r="O11" s="155" t="s">
         <v>519</v>
       </c>
     </row>
@@ -11969,10 +11998,10 @@
       <c r="M12" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N12" s="157" t="s">
+      <c r="N12" s="156" t="s">
         <v>569</v>
       </c>
-      <c r="O12" s="157" t="s">
+      <c r="O12" s="156" t="s">
         <v>519</v>
       </c>
     </row>
@@ -12016,10 +12045,10 @@
       <c r="M13" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N13" s="158" t="s">
+      <c r="N13" s="157" t="s">
         <v>570</v>
       </c>
-      <c r="O13" s="158" t="s">
+      <c r="O13" s="157" t="s">
         <v>519</v>
       </c>
     </row>
@@ -12063,10 +12092,10 @@
       <c r="M14" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N14" s="159" t="s">
+      <c r="N14" s="158" t="s">
         <v>571</v>
       </c>
-      <c r="O14" s="159" t="s">
+      <c r="O14" s="158" t="s">
         <v>519</v>
       </c>
     </row>
@@ -12110,10 +12139,10 @@
       <c r="M15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N15" s="160" t="s">
+      <c r="N15" s="159" t="s">
         <v>572</v>
       </c>
-      <c r="O15" s="160" t="s">
+      <c r="O15" s="159" t="s">
         <v>519</v>
       </c>
     </row>
@@ -12157,10 +12186,10 @@
       <c r="M16" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N16" s="161" t="s">
+      <c r="N16" s="160" t="s">
         <v>573</v>
       </c>
-      <c r="O16" s="161" t="s">
+      <c r="O16" s="160" t="s">
         <v>519</v>
       </c>
     </row>
@@ -12204,10 +12233,10 @@
       <c r="M17" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="N17" s="196" t="s">
+      <c r="N17" s="195" t="s">
         <v>335</v>
       </c>
-      <c r="O17" s="196" t="s">
+      <c r="O17" s="195" t="s">
         <v>590</v>
       </c>
     </row>
@@ -12251,10 +12280,10 @@
       <c r="M18" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="N18" s="197" t="s">
+      <c r="N18" s="196" t="s">
         <v>335</v>
       </c>
-      <c r="O18" s="197" t="s">
+      <c r="O18" s="196" t="s">
         <v>590</v>
       </c>
     </row>
@@ -12296,10 +12325,10 @@
       <c r="M19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N19" s="162" t="s">
+      <c r="N19" s="161" t="s">
         <v>335</v>
       </c>
-      <c r="O19" s="162" t="s">
+      <c r="O19" s="161" t="s">
         <v>574</v>
       </c>
     </row>
@@ -12343,10 +12372,10 @@
       <c r="M20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N20" s="163" t="s">
+      <c r="N20" s="162" t="s">
         <v>335</v>
       </c>
-      <c r="O20" s="163" t="s">
+      <c r="O20" s="162" t="s">
         <v>575</v>
       </c>
     </row>
@@ -12390,10 +12419,10 @@
       <c r="M21" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N21" s="164" t="s">
+      <c r="N21" s="163" t="s">
         <v>335</v>
       </c>
-      <c r="O21" s="164" t="s">
+      <c r="O21" s="163" t="s">
         <v>576</v>
       </c>
     </row>
@@ -12437,10 +12466,10 @@
       <c r="M22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N22" s="165" t="s">
+      <c r="N22" s="164" t="s">
         <v>335</v>
       </c>
-      <c r="O22" s="165" t="s">
+      <c r="O22" s="164" t="s">
         <v>352</v>
       </c>
     </row>
@@ -12482,10 +12511,10 @@
       <c r="M23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="N23" s="166" t="s">
+      <c r="N23" s="165" t="s">
         <v>335</v>
       </c>
-      <c r="O23" s="166" t="s">
+      <c r="O23" s="165" t="s">
         <v>577</v>
       </c>
     </row>
@@ -12527,10 +12556,10 @@
       <c r="M24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="N24" s="167" t="s">
+      <c r="N24" s="166" t="s">
         <v>335</v>
       </c>
-      <c r="O24" s="167" t="s">
+      <c r="O24" s="166" t="s">
         <v>578</v>
       </c>
     </row>
@@ -12574,10 +12603,10 @@
       <c r="M25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N25" s="168" t="s">
+      <c r="N25" s="167" t="s">
         <v>335</v>
       </c>
-      <c r="O25" s="168" t="s">
+      <c r="O25" s="167" t="s">
         <v>575</v>
       </c>
     </row>
@@ -12621,10 +12650,10 @@
       <c r="M26" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N26" s="169" t="s">
+      <c r="N26" s="168" t="s">
         <v>335</v>
       </c>
-      <c r="O26" s="169" t="s">
+      <c r="O26" s="168" t="s">
         <v>352</v>
       </c>
     </row>
@@ -12666,10 +12695,10 @@
       <c r="M27" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="N27" s="170" t="s">
+      <c r="N27" s="169" t="s">
         <v>335</v>
       </c>
-      <c r="O27" s="170" t="s">
+      <c r="O27" s="169" t="s">
         <v>579</v>
       </c>
     </row>
@@ -12713,10 +12742,10 @@
       <c r="M28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N28" s="171" t="s">
+      <c r="N28" s="170" t="s">
         <v>335</v>
       </c>
-      <c r="O28" s="171" t="s">
+      <c r="O28" s="170" t="s">
         <v>575</v>
       </c>
     </row>
@@ -12760,10 +12789,10 @@
       <c r="M29" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N29" s="172" t="s">
+      <c r="N29" s="171" t="s">
         <v>335</v>
       </c>
-      <c r="O29" s="172" t="s">
+      <c r="O29" s="171" t="s">
         <v>576</v>
       </c>
     </row>
@@ -12807,10 +12836,10 @@
       <c r="M30" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N30" s="173" t="s">
+      <c r="N30" s="172" t="s">
         <v>335</v>
       </c>
-      <c r="O30" s="173" t="s">
+      <c r="O30" s="172" t="s">
         <v>352</v>
       </c>
     </row>
@@ -12852,10 +12881,10 @@
       <c r="M31" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N31" s="174" t="s">
+      <c r="N31" s="173" t="s">
         <v>335</v>
       </c>
-      <c r="O31" s="174" t="s">
+      <c r="O31" s="173" t="s">
         <v>580</v>
       </c>
     </row>
@@ -12899,10 +12928,10 @@
       <c r="M32" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N32" s="175" t="s">
+      <c r="N32" s="174" t="s">
         <v>335</v>
       </c>
-      <c r="O32" s="175" t="s">
+      <c r="O32" s="174" t="s">
         <v>575</v>
       </c>
     </row>
@@ -12946,10 +12975,10 @@
       <c r="M33" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N33" s="176" t="s">
+      <c r="N33" s="175" t="s">
         <v>335</v>
       </c>
-      <c r="O33" s="176" t="s">
+      <c r="O33" s="175" t="s">
         <v>576</v>
       </c>
     </row>
@@ -12993,10 +13022,10 @@
       <c r="M34" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N34" s="177" t="s">
+      <c r="N34" s="176" t="s">
         <v>335</v>
       </c>
-      <c r="O34" s="177" t="s">
+      <c r="O34" s="176" t="s">
         <v>352</v>
       </c>
     </row>
@@ -13038,10 +13067,10 @@
       <c r="M35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="N35" s="178" t="s">
+      <c r="N35" s="177" t="s">
         <v>335</v>
       </c>
-      <c r="O35" s="178" t="s">
+      <c r="O35" s="177" t="s">
         <v>581</v>
       </c>
     </row>
@@ -13085,10 +13114,10 @@
       <c r="M36" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N36" s="179" t="s">
+      <c r="N36" s="178" t="s">
         <v>335</v>
       </c>
-      <c r="O36" s="179" t="s">
+      <c r="O36" s="178" t="s">
         <v>575</v>
       </c>
     </row>
@@ -13132,10 +13161,10 @@
       <c r="M37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N37" s="180" t="s">
+      <c r="N37" s="179" t="s">
         <v>335</v>
       </c>
-      <c r="O37" s="180" t="s">
+      <c r="O37" s="179" t="s">
         <v>351</v>
       </c>
     </row>
@@ -13179,10 +13208,10 @@
       <c r="M38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N38" s="181" t="s">
+      <c r="N38" s="180" t="s">
         <v>335</v>
       </c>
-      <c r="O38" s="181" t="s">
+      <c r="O38" s="180" t="s">
         <v>352</v>
       </c>
     </row>
@@ -13226,10 +13255,10 @@
       <c r="M39" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N39" s="182" t="s">
+      <c r="N39" s="181" t="s">
         <v>335</v>
       </c>
-      <c r="O39" s="182" t="s">
+      <c r="O39" s="181" t="s">
         <v>582</v>
       </c>
     </row>
@@ -13271,10 +13300,10 @@
       <c r="M40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N40" s="183" t="s">
+      <c r="N40" s="182" t="s">
         <v>335</v>
       </c>
-      <c r="O40" s="183" t="s">
+      <c r="O40" s="182" t="s">
         <v>583</v>
       </c>
     </row>
@@ -13318,10 +13347,10 @@
       <c r="M41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N41" s="184" t="s">
+      <c r="N41" s="183" t="s">
         <v>335</v>
       </c>
-      <c r="O41" s="184" t="s">
+      <c r="O41" s="183" t="s">
         <v>575</v>
       </c>
     </row>
@@ -13365,10 +13394,10 @@
       <c r="M42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N42" s="185" t="s">
+      <c r="N42" s="184" t="s">
         <v>335</v>
       </c>
-      <c r="O42" s="185" t="s">
+      <c r="O42" s="184" t="s">
         <v>351</v>
       </c>
     </row>
@@ -13412,10 +13441,10 @@
       <c r="M43" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N43" s="186" t="s">
+      <c r="N43" s="185" t="s">
         <v>335</v>
       </c>
-      <c r="O43" s="186" t="s">
+      <c r="O43" s="185" t="s">
         <v>352</v>
       </c>
     </row>
@@ -13457,10 +13486,10 @@
       <c r="M44" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N44" s="187" t="s">
+      <c r="N44" s="186" t="s">
         <v>335</v>
       </c>
-      <c r="O44" s="187" t="s">
+      <c r="O44" s="186" t="s">
         <v>584</v>
       </c>
     </row>
@@ -13504,10 +13533,10 @@
       <c r="M45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N45" s="188" t="s">
+      <c r="N45" s="187" t="s">
         <v>335</v>
       </c>
-      <c r="O45" s="188" t="s">
+      <c r="O45" s="187" t="s">
         <v>575</v>
       </c>
     </row>
@@ -13551,10 +13580,10 @@
       <c r="M46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N46" s="189" t="s">
+      <c r="N46" s="188" t="s">
         <v>335</v>
       </c>
-      <c r="O46" s="189" t="s">
+      <c r="O46" s="188" t="s">
         <v>585</v>
       </c>
     </row>
@@ -13598,10 +13627,10 @@
       <c r="M47" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N47" s="190" t="s">
+      <c r="N47" s="189" t="s">
         <v>335</v>
       </c>
-      <c r="O47" s="190" t="s">
+      <c r="O47" s="189" t="s">
         <v>585</v>
       </c>
     </row>
@@ -13645,10 +13674,10 @@
       <c r="M48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N48" s="191" t="s">
+      <c r="N48" s="190" t="s">
         <v>335</v>
       </c>
-      <c r="O48" s="191" t="s">
+      <c r="O48" s="190" t="s">
         <v>585</v>
       </c>
     </row>
@@ -13693,10 +13722,10 @@
       <c r="M49" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="N49" s="192" t="s">
+      <c r="N49" s="191" t="s">
         <v>335</v>
       </c>
-      <c r="O49" s="192" t="s">
+      <c r="O49" s="191" t="s">
         <v>586</v>
       </c>
     </row>
@@ -13738,10 +13767,10 @@
       <c r="M50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N50" s="193" t="s">
+      <c r="N50" s="192" t="s">
         <v>335</v>
       </c>
-      <c r="O50" s="193" t="s">
+      <c r="O50" s="192" t="s">
         <v>483</v>
       </c>
     </row>
@@ -13765,46 +13794,46 @@
       <c r="M51" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="N51" s="194" t="s">
+      <c r="N51" s="193" t="s">
         <v>335</v>
       </c>
-      <c r="O51" s="194" t="s">
+      <c r="O51" s="193" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="66"/>
-      <c r="B52" s="74" t="s">
+      <c r="A52" s="65"/>
+      <c r="B52" s="73" t="s">
         <v>434</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="65" t="s">
         <v>435</v>
       </c>
-      <c r="D52" s="66" t="s">
+      <c r="D52" s="65" t="s">
         <v>38</v>
       </c>
       <c r="E52" s="5">
         <v>30537</v>
       </c>
-      <c r="F52" s="66" t="s">
+      <c r="F52" s="65" t="s">
         <v>436</v>
       </c>
-      <c r="G52" s="66" t="s">
+      <c r="G52" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="H52" s="66" t="s">
+      <c r="H52" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="I52" s="66">
+      <c r="I52" s="65">
         <v>667875</v>
       </c>
       <c r="J52" s="8">
         <v>9996278123</v>
       </c>
-      <c r="K52" s="73" t="s">
+      <c r="K52" s="72" t="s">
         <v>560</v>
       </c>
-      <c r="L52" s="66" t="s">
+      <c r="L52" s="65" t="s">
         <v>110</v>
       </c>
       <c r="M52" s="1" t="s">
@@ -13961,7 +13990,7 @@
       <c r="J2" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K2" s="94" t="s">
+      <c r="K2" s="93" t="s">
         <v>486</v>
       </c>
     </row>
@@ -13996,7 +14025,7 @@
       <c r="J3" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K3" s="87" t="s">
+      <c r="K3" s="86" t="s">
         <v>486</v>
       </c>
     </row>
@@ -14031,7 +14060,7 @@
       <c r="J4" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K4" s="88" t="s">
+      <c r="K4" s="87" t="s">
         <v>486</v>
       </c>
     </row>
@@ -14066,7 +14095,7 @@
       <c r="J5" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K5" s="89" t="s">
+      <c r="K5" s="88" t="s">
         <v>486</v>
       </c>
     </row>
@@ -14101,7 +14130,7 @@
       <c r="J6" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K6" s="90" t="s">
+      <c r="K6" s="89" t="s">
         <v>486</v>
       </c>
     </row>
@@ -14136,7 +14165,7 @@
       <c r="J7" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K7" s="91" t="s">
+      <c r="K7" s="90" t="s">
         <v>486</v>
       </c>
     </row>
@@ -14171,7 +14200,7 @@
       <c r="J8" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="K8" s="92" t="s">
+      <c r="K8" s="91" t="s">
         <v>487</v>
       </c>
     </row>
@@ -14194,7 +14223,7 @@
       <c r="J9" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K9" s="93" t="s">
+      <c r="K9" s="92" t="s">
         <v>486</v>
       </c>
     </row>
@@ -14215,7 +14244,7 @@
       <c r="J10" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="K10" s="95" t="s">
+      <c r="K10" s="94" t="s">
         <v>488</v>
       </c>
     </row>
@@ -14238,7 +14267,7 @@
       <c r="J11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="K11" s="96" t="s">
+      <c r="K11" s="95" t="s">
         <v>351</v>
       </c>
     </row>
@@ -14261,7 +14290,7 @@
       <c r="J12" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="K12" s="97" t="s">
+      <c r="K12" s="96" t="s">
         <v>351</v>
       </c>
     </row>
@@ -14284,7 +14313,7 @@
       <c r="J13" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K13" s="98" t="s">
+      <c r="K13" s="97" t="s">
         <v>352</v>
       </c>
     </row>
@@ -14307,7 +14336,7 @@
       <c r="J14" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="K14" s="99" t="s">
+      <c r="K14" s="98" t="s">
         <v>489</v>
       </c>
     </row>
@@ -14330,7 +14359,7 @@
       <c r="J15" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="K15" s="100" t="s">
+      <c r="K15" s="99" t="s">
         <v>489</v>
       </c>
     </row>
@@ -14353,16 +14382,16 @@
       <c r="J16" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="K16" s="101" t="s">
+      <c r="K16" s="100" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="75" t="s">
+      <c r="A17" s="67"/>
+      <c r="B17" s="74" t="s">
         <v>437</v>
       </c>
-      <c r="C17" s="68">
+      <c r="C17" s="67">
         <v>12345</v>
       </c>
       <c r="J17" t="s">
@@ -14433,7 +14462,7 @@
       <c r="D2" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="198" t="s">
+      <c r="E2" s="197" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14450,7 +14479,7 @@
       <c r="D3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E3" s="199" t="s">
+      <c r="E3" s="198" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14467,7 +14496,7 @@
       <c r="D4" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E4" s="200" t="s">
+      <c r="E4" s="199" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14484,7 +14513,7 @@
       <c r="D5" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="201" t="s">
+      <c r="E5" s="200" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14501,7 +14530,7 @@
       <c r="D6" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E6" s="202" t="s">
+      <c r="E6" s="201" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14518,7 +14547,7 @@
       <c r="D7" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="203" t="s">
+      <c r="E7" s="202" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14535,7 +14564,7 @@
       <c r="D8" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E8" s="204" t="s">
+      <c r="E8" s="203" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14552,7 +14581,7 @@
       <c r="D9" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E9" s="205" t="s">
+      <c r="E9" s="204" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14569,7 +14598,7 @@
       <c r="D10" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E10" s="206" t="s">
+      <c r="E10" s="205" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14586,7 +14615,7 @@
       <c r="D11" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E11" s="207" t="s">
+      <c r="E11" s="206" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14603,7 +14632,7 @@
       <c r="D12" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E12" s="208" t="s">
+      <c r="E12" s="207" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14620,7 +14649,7 @@
       <c r="D13" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E13" s="209" t="s">
+      <c r="E13" s="208" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14637,7 +14666,7 @@
       <c r="D14" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E14" s="210" t="s">
+      <c r="E14" s="209" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14654,7 +14683,7 @@
       <c r="D15" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E15" s="211" t="s">
+      <c r="E15" s="210" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14671,7 +14700,7 @@
       <c r="D16" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E16" s="212" t="s">
+      <c r="E16" s="211" t="s">
         <v>591</v>
       </c>
     </row>
@@ -14686,7 +14715,7 @@
       <c r="D17" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E17" s="213" t="s">
+      <c r="E17" s="212" t="s">
         <v>488</v>
       </c>
     </row>
@@ -14703,7 +14732,7 @@
       <c r="D18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="214" t="s">
+      <c r="E18" s="213" t="s">
         <v>351</v>
       </c>
     </row>
@@ -14720,7 +14749,7 @@
       <c r="D19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="215" t="s">
+      <c r="E19" s="214" t="s">
         <v>351</v>
       </c>
     </row>
@@ -14737,7 +14766,7 @@
       <c r="D20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="216" t="s">
+      <c r="E20" s="215" t="s">
         <v>352</v>
       </c>
     </row>
@@ -14754,7 +14783,7 @@
       <c r="D21" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E21" s="217" t="s">
+      <c r="E21" s="216" t="s">
         <v>592</v>
       </c>
     </row>
@@ -14771,7 +14800,7 @@
       <c r="D22" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E22" s="218" t="s">
+      <c r="E22" s="217" t="s">
         <v>592</v>
       </c>
     </row>
@@ -14788,7 +14817,7 @@
       <c r="D23" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E23" s="219" t="s">
+      <c r="E23" s="218" t="s">
         <v>592</v>
       </c>
     </row>
@@ -14799,13 +14828,13 @@
       <c r="B24" s="59" t="s">
         <v>322</v>
       </c>
-      <c r="C24" s="102">
+      <c r="C24" s="101">
         <v>96501</v>
       </c>
       <c r="D24" s="52" t="s">
         <v>294</v>
       </c>
-      <c r="E24" s="220" t="s">
+      <c r="E24" s="219" t="s">
         <v>593</v>
       </c>
     </row>
@@ -14813,38 +14842,38 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="147" t="s">
+      <c r="B25" s="146" t="s">
         <v>363</v>
       </c>
-      <c r="C25" s="143">
+      <c r="C25" s="142">
         <v>37672</v>
       </c>
-      <c r="D25" s="144" t="s">
+      <c r="D25" s="143" t="s">
         <v>255</v>
       </c>
-      <c r="E25" s="221" t="s">
+      <c r="E25" s="220" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="76"/>
-      <c r="B26" s="146" t="s">
+      <c r="A26" s="75"/>
+      <c r="B26" s="145" t="s">
         <v>438</v>
       </c>
-      <c r="C26" s="76">
+      <c r="C26" s="75">
         <v>12345</v>
       </c>
       <c r="D26" s="50" t="s">
         <v>285</v>
       </c>
-      <c r="E26" s="145"/>
+      <c r="E26" s="144"/>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="51"/>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
-      <c r="E27" s="145"/>
+      <c r="E27" s="144"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14861,7 +14890,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14909,7 +14938,7 @@
       <c r="B2" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="71">
         <v>73735</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -14921,10 +14950,10 @@
       <c r="F2" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G2" s="295" t="s">
+      <c r="G2" s="294" t="s">
         <v>627</v>
       </c>
-      <c r="H2" s="295" t="s">
+      <c r="H2" s="294" t="s">
         <v>507</v>
       </c>
     </row>
@@ -14935,7 +14964,7 @@
       <c r="B3" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C3" s="72">
+      <c r="C3" s="71">
         <v>37705</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -14947,10 +14976,10 @@
       <c r="F3" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G3" s="296" t="s">
+      <c r="G3" s="295" t="s">
         <v>628</v>
       </c>
-      <c r="H3" s="296" t="s">
+      <c r="H3" s="295" t="s">
         <v>507</v>
       </c>
     </row>
@@ -14961,7 +14990,7 @@
       <c r="B4" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="71">
         <v>73735</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -14973,10 +15002,10 @@
       <c r="F4" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G4" s="297" t="s">
+      <c r="G4" s="296" t="s">
         <v>629</v>
       </c>
-      <c r="H4" s="297" t="s">
+      <c r="H4" s="296" t="s">
         <v>507</v>
       </c>
     </row>
@@ -14987,7 +15016,7 @@
       <c r="B5" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="71">
         <v>37705</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -14999,10 +15028,10 @@
       <c r="F5" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G5" s="298" t="s">
+      <c r="G5" s="297" t="s">
         <v>630</v>
       </c>
-      <c r="H5" s="298" t="s">
+      <c r="H5" s="297" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15013,7 +15042,7 @@
       <c r="B6" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C6" s="102">
+      <c r="C6" s="101">
         <v>73735</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -15025,10 +15054,10 @@
       <c r="F6" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G6" s="299" t="s">
+      <c r="G6" s="298" t="s">
         <v>631</v>
       </c>
-      <c r="H6" s="299" t="s">
+      <c r="H6" s="298" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15039,7 +15068,7 @@
       <c r="B7" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C7" s="102">
+      <c r="C7" s="101">
         <v>73735</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -15051,10 +15080,10 @@
       <c r="F7" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G7" s="300" t="s">
+      <c r="G7" s="299" t="s">
         <v>632</v>
       </c>
-      <c r="H7" s="300" t="s">
+      <c r="H7" s="299" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15065,7 +15094,7 @@
       <c r="B8" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C8" s="71">
         <v>73735</v>
       </c>
       <c r="D8" s="1"/>
@@ -15075,10 +15104,10 @@
       <c r="F8" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G8" s="301" t="s">
+      <c r="G8" s="300" t="s">
         <v>633</v>
       </c>
-      <c r="H8" s="301" t="s">
+      <c r="H8" s="300" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15089,7 +15118,7 @@
       <c r="B9" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="71">
         <v>98487</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -15101,10 +15130,10 @@
       <c r="F9" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G9" s="302" t="s">
+      <c r="G9" s="301" t="s">
         <v>634</v>
       </c>
-      <c r="H9" s="302" t="s">
+      <c r="H9" s="301" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15115,7 +15144,7 @@
       <c r="B10" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C10" s="72">
+      <c r="C10" s="71">
         <v>98487</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -15127,10 +15156,10 @@
       <c r="F10" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G10" s="222" t="s">
+      <c r="G10" s="221" t="s">
         <v>597</v>
       </c>
-      <c r="H10" s="222" t="s">
+      <c r="H10" s="221" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15141,7 +15170,7 @@
       <c r="B11" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C11" s="72">
+      <c r="C11" s="71">
         <v>98487</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -15153,10 +15182,10 @@
       <c r="F11" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G11" s="105" t="s">
+      <c r="G11" s="104" t="s">
         <v>511</v>
       </c>
-      <c r="H11" s="105" t="s">
+      <c r="H11" s="104" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15167,7 +15196,7 @@
       <c r="B12" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C12" s="72">
+      <c r="C12" s="71">
         <v>37705</v>
       </c>
       <c r="D12" s="54" t="s">
@@ -15179,10 +15208,10 @@
       <c r="F12" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G12" s="106" t="s">
+      <c r="G12" s="105" t="s">
         <v>512</v>
       </c>
-      <c r="H12" s="106" t="s">
+      <c r="H12" s="105" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15193,7 +15222,7 @@
       <c r="B13" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C13" s="71">
         <v>37705</v>
       </c>
       <c r="D13" s="54" t="s">
@@ -15205,10 +15234,10 @@
       <c r="F13" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G13" s="107" t="s">
+      <c r="G13" s="106" t="s">
         <v>513</v>
       </c>
-      <c r="H13" s="107" t="s">
+      <c r="H13" s="106" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15219,7 +15248,7 @@
       <c r="B14" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C14" s="72">
+      <c r="C14" s="71">
         <v>37705</v>
       </c>
       <c r="D14" s="54" t="s">
@@ -15231,10 +15260,10 @@
       <c r="F14" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G14" s="108" t="s">
+      <c r="G14" s="107" t="s">
         <v>514</v>
       </c>
-      <c r="H14" s="108" t="s">
+      <c r="H14" s="107" t="s">
         <v>507</v>
       </c>
     </row>
@@ -15255,10 +15284,10 @@
       <c r="F15" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G15" s="109" t="s">
+      <c r="G15" s="108" t="s">
         <v>335</v>
       </c>
-      <c r="H15" s="109" t="s">
+      <c r="H15" s="108" t="s">
         <v>515</v>
       </c>
     </row>
@@ -15281,10 +15310,10 @@
       <c r="F16" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G16" s="110" t="s">
+      <c r="G16" s="109" t="s">
         <v>335</v>
       </c>
-      <c r="H16" s="110" t="s">
+      <c r="H16" s="109" t="s">
         <v>515</v>
       </c>
     </row>
@@ -15307,10 +15336,10 @@
       <c r="F17" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G17" s="111" t="s">
+      <c r="G17" s="110" t="s">
         <v>335</v>
       </c>
-      <c r="H17" s="111" t="s">
+      <c r="H17" s="110" t="s">
         <v>515</v>
       </c>
     </row>
@@ -15333,10 +15362,10 @@
       <c r="F18" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G18" s="112" t="s">
+      <c r="G18" s="111" t="s">
         <v>335</v>
       </c>
-      <c r="H18" s="112" t="s">
+      <c r="H18" s="111" t="s">
         <v>515</v>
       </c>
     </row>
@@ -15359,10 +15388,10 @@
       <c r="F19" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G19" s="113" t="s">
+      <c r="G19" s="112" t="s">
         <v>335</v>
       </c>
-      <c r="H19" s="113" t="s">
+      <c r="H19" s="112" t="s">
         <v>515</v>
       </c>
     </row>
@@ -15373,7 +15402,7 @@
       <c r="B20" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C20" s="72">
+      <c r="C20" s="71">
         <v>98487</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -15383,10 +15412,10 @@
       <c r="F20" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G20" s="114" t="s">
+      <c r="G20" s="113" t="s">
         <v>335</v>
       </c>
-      <c r="H20" s="114" t="s">
+      <c r="H20" s="113" t="s">
         <v>516</v>
       </c>
     </row>
@@ -15397,7 +15426,7 @@
       <c r="B21" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C21" s="72">
+      <c r="C21" s="71">
         <v>98487</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -15409,10 +15438,10 @@
       <c r="F21" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G21" s="115" t="s">
+      <c r="G21" s="114" t="s">
         <v>335</v>
       </c>
-      <c r="H21" s="115" t="s">
+      <c r="H21" s="114" t="s">
         <v>516</v>
       </c>
     </row>
@@ -15423,7 +15452,7 @@
       <c r="B22" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C22" s="72">
+      <c r="C22" s="71">
         <v>98487</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -15435,10 +15464,10 @@
       <c r="F22" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G22" s="116" t="s">
+      <c r="G22" s="115" t="s">
         <v>335</v>
       </c>
-      <c r="H22" s="116" t="s">
+      <c r="H22" s="115" t="s">
         <v>516</v>
       </c>
     </row>
@@ -15449,7 +15478,7 @@
       <c r="B23" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C23" s="72">
+      <c r="C23" s="71">
         <v>98487</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -15461,10 +15490,10 @@
       <c r="F23" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G23" s="117" t="s">
+      <c r="G23" s="116" t="s">
         <v>335</v>
       </c>
-      <c r="H23" s="117" t="s">
+      <c r="H23" s="116" t="s">
         <v>516</v>
       </c>
     </row>
@@ -15475,7 +15504,7 @@
       <c r="B24" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C24" s="72">
+      <c r="C24" s="71">
         <v>98487</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -15487,10 +15516,10 @@
       <c r="F24" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G24" s="118" t="s">
+      <c r="G24" s="117" t="s">
         <v>335</v>
       </c>
-      <c r="H24" s="118" t="s">
+      <c r="H24" s="117" t="s">
         <v>516</v>
       </c>
     </row>
@@ -15501,7 +15530,7 @@
       <c r="B25" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="71">
         <v>98487</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -15513,10 +15542,10 @@
       <c r="F25" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G25" s="119" t="s">
+      <c r="G25" s="118" t="s">
         <v>335</v>
       </c>
-      <c r="H25" s="119" t="s">
+      <c r="H25" s="118" t="s">
         <v>516</v>
       </c>
     </row>
@@ -15533,10 +15562,10 @@
       <c r="F26" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G26" s="120" t="s">
+      <c r="G26" s="119" t="s">
         <v>335</v>
       </c>
-      <c r="H26" s="120" t="s">
+      <c r="H26" s="119" t="s">
         <v>515</v>
       </c>
     </row>
@@ -15547,22 +15576,22 @@
       <c r="B27" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C27" s="66">
+      <c r="C27" s="65">
         <v>37672</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="65" t="s">
         <v>445</v>
       </c>
-      <c r="E27" s="66">
+      <c r="E27" s="65">
         <v>1000</v>
       </c>
-      <c r="F27" s="66" t="s">
+      <c r="F27" s="65" t="s">
         <v>503</v>
       </c>
-      <c r="G27" s="121" t="s">
+      <c r="G27" s="120" t="s">
         <v>335</v>
       </c>
-      <c r="H27" s="121" t="s">
+      <c r="H27" s="120" t="s">
         <v>515</v>
       </c>
     </row>
@@ -15626,7 +15655,7 @@
       <c r="E2" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="F2" s="247"/>
+      <c r="F2" s="246"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -15642,7 +15671,7 @@
       <c r="E3" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="F3" s="248"/>
+      <c r="F3" s="247"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -15658,7 +15687,7 @@
       <c r="E4" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="F4" s="249"/>
+      <c r="F4" s="248"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -15676,7 +15705,7 @@
       <c r="E5" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="F5" s="250"/>
+      <c r="F5" s="249"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -15694,7 +15723,7 @@
       <c r="E6" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F6" s="251"/>
+      <c r="F6" s="250"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -15708,7 +15737,7 @@
       <c r="E7" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="F7" s="252"/>
+      <c r="F7" s="251"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -15724,7 +15753,7 @@
       <c r="E8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="253"/>
+      <c r="F8" s="252"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -15740,7 +15769,7 @@
       <c r="E9" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="254"/>
+      <c r="F9" s="253"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -15756,7 +15785,7 @@
       <c r="E10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="255"/>
+      <c r="F10" s="254"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -15765,14 +15794,14 @@
       <c r="B11" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="64">
         <v>44435</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F11" s="256"/>
+      <c r="F11" s="255"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -15788,7 +15817,7 @@
       <c r="E12" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F12" s="257"/>
+      <c r="F12" s="256"/>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -15804,7 +15833,7 @@
       <c r="E13" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F13" s="258"/>
+      <c r="F13" s="257"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15859,7 +15888,7 @@
       <c r="D2" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="121" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15874,7 +15903,7 @@
       <c r="D3" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="122" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15889,7 +15918,7 @@
       <c r="D4" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E4" s="124" t="s">
+      <c r="E4" s="123" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15904,7 +15933,7 @@
       <c r="D5" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E5" s="125" t="s">
+      <c r="E5" s="124" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15919,7 +15948,7 @@
       <c r="D6" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E6" s="126" t="s">
+      <c r="E6" s="125" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15934,7 +15963,7 @@
       <c r="D7" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E7" s="127" t="s">
+      <c r="E7" s="126" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15949,7 +15978,7 @@
       <c r="D8" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E8" s="128" t="s">
+      <c r="E8" s="127" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15964,7 +15993,7 @@
       <c r="D9" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E9" s="129" t="s">
+      <c r="E9" s="128" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15979,7 +16008,7 @@
       <c r="D10" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E10" s="130" t="s">
+      <c r="E10" s="129" t="s">
         <v>505</v>
       </c>
     </row>
@@ -15996,7 +16025,7 @@
       <c r="D11" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E11" s="131" t="s">
+      <c r="E11" s="130" t="s">
         <v>505</v>
       </c>
     </row>
@@ -16013,7 +16042,7 @@
       <c r="D12" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E12" s="132" t="s">
+      <c r="E12" s="131" t="s">
         <v>505</v>
       </c>
     </row>
@@ -16030,7 +16059,7 @@
       <c r="D13" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E13" s="133" t="s">
+      <c r="E13" s="132" t="s">
         <v>505</v>
       </c>
     </row>
@@ -16047,7 +16076,7 @@
       <c r="D14" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E14" s="134" t="s">
+      <c r="E14" s="133" t="s">
         <v>505</v>
       </c>
     </row>
@@ -16064,7 +16093,7 @@
       <c r="D15" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E15" s="135" t="s">
+      <c r="E15" s="134" t="s">
         <v>350</v>
       </c>
     </row>
@@ -16081,7 +16110,7 @@
       <c r="D16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="136" t="s">
+      <c r="E16" s="135" t="s">
         <v>351</v>
       </c>
     </row>
@@ -16098,7 +16127,7 @@
       <c r="D17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="137" t="s">
+      <c r="E17" s="136" t="s">
         <v>351</v>
       </c>
     </row>
@@ -16115,7 +16144,7 @@
       <c r="D18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="138" t="s">
+      <c r="E18" s="137" t="s">
         <v>352</v>
       </c>
     </row>
@@ -16132,7 +16161,7 @@
       <c r="D19" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E19" s="139" t="s">
+      <c r="E19" s="138" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16149,7 +16178,7 @@
       <c r="D20" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E20" s="140" t="s">
+      <c r="E20" s="139" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16166,7 +16195,7 @@
       <c r="D21" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E21" s="141" t="s">
+      <c r="E21" s="140" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16195,7 +16224,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16257,7 +16286,7 @@
       <c r="H2" s="49" t="s">
         <v>596</v>
       </c>
-      <c r="I2" s="265" t="s">
+      <c r="I2" s="264" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16282,7 +16311,7 @@
       <c r="H3" s="49" t="s">
         <v>611</v>
       </c>
-      <c r="I3" s="266" t="s">
+      <c r="I3" s="265" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16290,7 +16319,7 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="65" t="s">
         <v>391</v>
       </c>
       <c r="C4" s="1"/>
@@ -16307,7 +16336,7 @@
       <c r="H4" s="49" t="s">
         <v>612</v>
       </c>
-      <c r="I4" s="267" t="s">
+      <c r="I4" s="266" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16315,7 +16344,7 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="65" t="s">
         <v>379</v>
       </c>
       <c r="C5" s="48"/>
@@ -16332,7 +16361,7 @@
       <c r="H5" s="49" t="s">
         <v>598</v>
       </c>
-      <c r="I5" s="268" t="s">
+      <c r="I5" s="267" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16340,7 +16369,7 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="65" t="s">
         <v>380</v>
       </c>
       <c r="C6" s="48"/>
@@ -16357,7 +16386,7 @@
       <c r="H6" s="49" t="s">
         <v>613</v>
       </c>
-      <c r="I6" s="269" t="s">
+      <c r="I6" s="268" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16365,7 +16394,7 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="65" t="s">
         <v>381</v>
       </c>
       <c r="C7" s="1"/>
@@ -16382,7 +16411,7 @@
       <c r="H7" s="49" t="s">
         <v>614</v>
       </c>
-      <c r="I7" s="270" t="s">
+      <c r="I7" s="269" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16390,7 +16419,7 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="65" t="s">
         <v>383</v>
       </c>
       <c r="C8" s="1"/>
@@ -16407,7 +16436,7 @@
       <c r="H8" s="49" t="s">
         <v>610</v>
       </c>
-      <c r="I8" s="271" t="s">
+      <c r="I8" s="270" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16415,7 +16444,7 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="65" t="s">
         <v>377</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -16434,7 +16463,7 @@
       <c r="H9" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I9" s="271" t="s">
+      <c r="I9" s="270" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16461,7 +16490,7 @@
       <c r="H10" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I10" s="223" t="s">
+      <c r="I10" s="222" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16490,7 +16519,7 @@
       <c r="H11" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I11" s="224" t="s">
+      <c r="I11" s="223" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16519,7 +16548,7 @@
       <c r="H12" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I12" s="225" t="s">
+      <c r="I12" s="224" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16548,7 +16577,7 @@
       <c r="H13" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I13" s="226" t="s">
+      <c r="I13" s="225" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16577,7 +16606,7 @@
       <c r="H14" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I14" s="227" t="s">
+      <c r="I14" s="226" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16606,7 +16635,7 @@
       <c r="H15" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I15" s="228" t="s">
+      <c r="I15" s="227" t="s">
         <v>353</v>
       </c>
     </row>
@@ -16614,7 +16643,7 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="65" t="s">
         <v>372</v>
       </c>
       <c r="C16" s="1">
@@ -16631,7 +16660,7 @@
       <c r="H16" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I16" s="230" t="s">
+      <c r="I16" s="229" t="s">
         <v>602</v>
       </c>
     </row>
@@ -16639,7 +16668,7 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>373</v>
       </c>
       <c r="C17" s="1">
@@ -16658,7 +16687,7 @@
       <c r="H17" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I17" s="231" t="s">
+      <c r="I17" s="230" t="s">
         <v>602</v>
       </c>
     </row>
@@ -16666,7 +16695,7 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="65" t="s">
         <v>374</v>
       </c>
       <c r="C18" s="1">
@@ -16685,7 +16714,7 @@
       <c r="H18" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I18" s="232" t="s">
+      <c r="I18" s="231" t="s">
         <v>602</v>
       </c>
     </row>
@@ -16693,7 +16722,7 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="65" t="s">
         <v>375</v>
       </c>
       <c r="C19" s="1">
@@ -16712,7 +16741,7 @@
       <c r="H19" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I19" s="233" t="s">
+      <c r="I19" s="232" t="s">
         <v>602</v>
       </c>
     </row>
@@ -16720,7 +16749,7 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="65" t="s">
         <v>385</v>
       </c>
       <c r="C20" s="1"/>
@@ -16733,7 +16762,7 @@
       <c r="H20" s="49" t="s">
         <v>599</v>
       </c>
-      <c r="I20" s="229" t="s">
+      <c r="I20" s="228" t="s">
         <v>353</v>
       </c>
     </row>

</xml_diff>